<commit_message>
Lookup exercise Sept 17 9.34pm
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\Documents\NSS-DA13\Excel\lookups-exercise-RenukaD13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B674FEA7-32CF-479B-83A7-589E48A727F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -314,7 +314,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,7 +458,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -809,7 +809,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,6 +819,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -880,9 +885,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -920,7 +925,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1026,7 +1031,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1168,7 +1173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1176,27 +1181,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
-    <col min="14" max="15" width="17.85546875" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="15.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
+    <col min="14" max="15" width="17.81640625" customWidth="1"/>
+    <col min="16" max="17" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1212,7 +1217,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1246,7 +1251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1256,23 +1261,56 @@
       <c r="C2">
         <v>341243679.13</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>-15396420.870000005</v>
+      </c>
+      <c r="E2" s="5">
+        <f>IFERROR(D2/B2,0)</f>
+        <v>-4.3170750765267295E-2</v>
+      </c>
+      <c r="F2" s="9">
+        <f>RANK(E2,$E$2:$E$52,1)</f>
+        <v>14</v>
+      </c>
       <c r="G2">
         <v>382685200</v>
       </c>
       <c r="H2">
         <v>346340810.81999999</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="I2">
+        <f>H2-G2</f>
+        <v>-36344389.180000007</v>
+      </c>
+      <c r="J2" s="5">
+        <f>IFERROR(I2/H2,0)</f>
+        <v>-0.10493822282725118</v>
+      </c>
+      <c r="K2">
+        <f>RANK(J2,$J$2:$J$52,1)</f>
+        <v>10</v>
+      </c>
       <c r="L2">
         <v>376548600</v>
       </c>
       <c r="M2">
         <v>355279492.22999901</v>
       </c>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2">
+        <f>M2-L2</f>
+        <v>-21269107.770000994</v>
+      </c>
+      <c r="O2" s="5">
+        <f>IFERROR(N2/L2,0)</f>
+        <v>-5.6484362894991494E-2</v>
+      </c>
+      <c r="P2">
+        <f>RANK(O2,$O$2:$O$52,1)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1282,23 +1320,56 @@
       <c r="C3">
         <v>321214.59000000003</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="D3">
+        <f>C3-B3</f>
+        <v>-7585.4099999999744</v>
+      </c>
+      <c r="E3" s="5">
+        <f>IFERROR(D3/B3,0)</f>
+        <v>-2.3069981751824741E-2</v>
+      </c>
+      <c r="F3" s="9">
+        <f>RANK(E3,$E$2:$E$52,1)</f>
+        <v>22</v>
+      </c>
       <c r="G3">
         <v>334800</v>
       </c>
       <c r="H3">
         <v>312433.70999999897</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="I3">
+        <f>H3-G3</f>
+        <v>-22366.290000001027</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J52" si="0">IFERROR(I3/H3,0)</f>
+        <v>-7.1587313673678488E-2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K52" si="1">RANK(J3,$J$2:$J$52,1)</f>
+        <v>14</v>
+      </c>
       <c r="L3">
         <v>322700</v>
       </c>
       <c r="M3">
         <v>322263.03999999998</v>
       </c>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="N3">
+        <f t="shared" ref="N3:N52" si="2">M3-L3</f>
+        <v>-436.96000000002095</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O52" si="3">IFERROR(N3/L3,0)</f>
+        <v>-1.3540749922529313E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P52" si="4">RANK(O3,$O$2:$O$52,1)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1308,23 +1379,56 @@
       <c r="C4">
         <v>3115157.5599999898</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="D4">
+        <f>C4-B4</f>
+        <v>-15442.440000010189</v>
+      </c>
+      <c r="E4" s="5">
+        <f>IFERROR(D4/B4,0)</f>
+        <v>-4.9327413275443007E-3</v>
+      </c>
+      <c r="F4" s="9">
+        <f>RANK(E4,$E$2:$E$52,1)</f>
+        <v>42</v>
+      </c>
       <c r="G4">
         <v>3652300</v>
       </c>
       <c r="H4">
         <v>3589693.2099999902</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="I4">
+        <f>H4-G4</f>
+        <v>-62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.7440707697694863E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
       <c r="L4">
         <v>3662400</v>
       </c>
       <c r="M4">
         <v>3564983.04999999</v>
       </c>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>-97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1334,23 +1438,56 @@
       <c r="C5">
         <v>6947552.6699999999</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="D5">
+        <f>C5-B5</f>
+        <v>-723147.33000000007</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IFERROR(D5/B5,0)</f>
+        <v>-9.4273968477453174E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <f>RANK(E5,$E$2:$E$52,1)</f>
+        <v>4</v>
+      </c>
       <c r="G5">
         <v>7968300</v>
       </c>
       <c r="H5">
         <v>7020609.3200000003</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="I5">
+        <f>H5-G5</f>
+        <v>-947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.13498695580457107</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="L5">
         <v>7759600</v>
       </c>
       <c r="M5">
         <v>7497322.9100000001</v>
       </c>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>-262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1360,23 +1497,56 @@
       <c r="C6">
         <v>385908.52</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="D6">
+        <f>C6-B6</f>
+        <v>-23391.479999999981</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IFERROR(D6/B6,0)</f>
+        <v>-5.7149963352064452E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <f>RANK(E6,$E$2:$E$52,1)</f>
+        <v>11</v>
+      </c>
       <c r="G6">
         <v>428500</v>
       </c>
       <c r="H6">
         <v>427758.64</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="I6">
+        <f>H6-G6</f>
+        <v>-741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.7331268866947632E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
       <c r="L6">
         <v>445200</v>
       </c>
       <c r="M6">
         <v>445114.28999999899</v>
       </c>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>-85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1386,23 +1556,56 @@
       <c r="C7">
         <v>2946071.21</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="D7">
+        <f>C7-B7</f>
+        <v>-382928.79000000004</v>
+      </c>
+      <c r="E7" s="5">
+        <f>IFERROR(D7/B7,0)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F7" s="9">
+        <f>RANK(E7,$E$2:$E$52,1)</f>
+        <v>2</v>
+      </c>
       <c r="G7">
         <v>3390900</v>
       </c>
       <c r="H7">
         <v>3051483.41</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="I7">
+        <f>H7-G7</f>
+        <v>-339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.11123002959403271</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
       <c r="L7">
         <v>3345200</v>
       </c>
       <c r="M7">
         <v>2946440.08</v>
       </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>-398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1412,23 +1615,56 @@
       <c r="C8">
         <v>1315623.30999999</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="D8">
+        <f>C8-B8</f>
+        <v>-236476.69000000996</v>
+      </c>
+      <c r="E8" s="5">
+        <f>IFERROR(D8/B8,0)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="F8" s="9">
+        <f>RANK(E8,$E$2:$E$52,1)</f>
+        <v>1</v>
+      </c>
       <c r="G8">
         <v>1590700</v>
       </c>
       <c r="H8">
         <v>1383905.98999999</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="I8">
+        <f>H8-G8</f>
+        <v>-206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.14942778736004425</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="L8">
         <v>1579300</v>
       </c>
       <c r="M8">
         <v>1337735.3199999901</v>
       </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>-241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1438,23 +1674,56 @@
       <c r="C9">
         <v>8952825.2799999993</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="D9">
+        <f>C9-B9</f>
+        <v>-396574.72000000067</v>
+      </c>
+      <c r="E9" s="5">
+        <f>IFERROR(D9/B9,0)</f>
+        <v>-4.2417130511048909E-2</v>
+      </c>
+      <c r="F9" s="9">
+        <f>RANK(E9,$E$2:$E$52,1)</f>
+        <v>16</v>
+      </c>
       <c r="G9">
         <v>11073700</v>
       </c>
       <c r="H9">
         <v>9929059.5199999996</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="I9">
+        <f>H9-G9</f>
+        <v>-1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.11528186307014912</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="L9">
         <v>10790500</v>
       </c>
       <c r="M9">
         <v>9993599.52999999</v>
       </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>-796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="3"/>
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1464,23 +1733,56 @@
       <c r="C10">
         <v>407090.37</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="D10">
+        <f>C10-B10</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="E10" s="5">
+        <f>IFERROR(D10/B10,0)</f>
+        <v>-8.1681998646514792E-2</v>
+      </c>
+      <c r="F10" s="9">
+        <f>RANK(E10,$E$2:$E$52,1)</f>
+        <v>6</v>
+      </c>
       <c r="G10">
         <v>495200</v>
       </c>
       <c r="H10">
         <v>467907.84000000003</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="I10">
+        <f>H10-G10</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.8328067339072524E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
       <c r="L10">
         <v>487500</v>
       </c>
       <c r="M10">
         <v>478318.92</v>
       </c>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1490,23 +1792,56 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="D11">
+        <f>C11-B11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f>IFERROR(D11/B11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <f>RANK(E11,$E$2:$E$52,1)</f>
+        <v>47</v>
+      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="I11">
+        <f>H11-G11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="L11">
         <v>375000</v>
       </c>
       <c r="M11">
         <v>63771.91</v>
       </c>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1516,23 +1851,56 @@
       <c r="C12">
         <v>4066595.33</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="D12">
+        <f>C12-B12</f>
+        <v>-214304.66999999993</v>
+      </c>
+      <c r="E12" s="5">
+        <f>IFERROR(D12/B12,0)</f>
+        <v>-5.0060657805601608E-2</v>
+      </c>
+      <c r="F12" s="9">
+        <f>RANK(E12,$E$2:$E$52,1)</f>
+        <v>13</v>
+      </c>
       <c r="G12">
         <v>4700400</v>
       </c>
       <c r="H12">
         <v>4205555.5999999996</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="I12">
+        <f>H12-G12</f>
+        <v>-494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.11766445318188171</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
       <c r="L12">
         <v>4677800</v>
       </c>
       <c r="M12">
         <v>4371713.1399999997</v>
       </c>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>-306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1542,23 +1910,56 @@
       <c r="C13">
         <v>5772288.3300000001</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="D13">
+        <f>C13-B13</f>
+        <v>-75511.669999999925</v>
+      </c>
+      <c r="E13" s="5">
+        <f>IFERROR(D13/B13,0)</f>
+        <v>-1.2912833886247806E-2</v>
+      </c>
+      <c r="F13" s="9">
+        <f>RANK(E13,$E$2:$E$52,1)</f>
+        <v>33</v>
+      </c>
       <c r="G13">
         <v>6223700</v>
       </c>
       <c r="H13">
         <v>5909077.9399999902</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="I13">
+        <f>H13-G13</f>
+        <v>-314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.3243850088734883E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
       <c r="L13">
         <v>6207300</v>
       </c>
       <c r="M13">
         <v>6056976.6699999999</v>
       </c>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>-150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1568,23 +1969,56 @@
       <c r="C14">
         <v>505017.37</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="D14">
+        <f>C14-B14</f>
+        <v>-6982.6300000000047</v>
+      </c>
+      <c r="E14" s="5">
+        <f>IFERROR(D14/B14,0)</f>
+        <v>-1.3637949218750009E-2</v>
+      </c>
+      <c r="F14" s="9">
+        <f>RANK(E14,$E$2:$E$52,1)</f>
+        <v>30</v>
+      </c>
       <c r="G14">
         <v>530500</v>
       </c>
       <c r="H14">
         <v>524402.98</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="I14">
+        <f>H14-G14</f>
+        <v>-6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.1626592968636483E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
       <c r="L14">
         <v>526200</v>
       </c>
       <c r="M14">
         <v>504989.88</v>
       </c>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>-21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1594,23 +2028,56 @@
       <c r="C15">
         <v>156545919.90000001</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="D15">
+        <f>C15-B15</f>
+        <v>496819.90000000596</v>
+      </c>
+      <c r="E15" s="5">
+        <f>IFERROR(D15/B15,0)</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="F15" s="9">
+        <f>RANK(E15,$E$2:$E$52,1)</f>
+        <v>51</v>
+      </c>
       <c r="G15">
         <v>184167800</v>
       </c>
       <c r="H15">
         <v>175966389.24999899</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="I15">
+        <f>H15-G15</f>
+        <v>-8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.6607825420280143E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
       <c r="L15">
         <v>188953500</v>
       </c>
       <c r="M15">
         <v>184450910.84999901</v>
       </c>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>-4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1620,23 +2087,56 @@
       <c r="C16">
         <v>6522480.4599999897</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="D16">
+        <f>C16-B16</f>
+        <v>-78219.540000010282</v>
+      </c>
+      <c r="E16" s="5">
+        <f>IFERROR(D16/B16,0)</f>
+        <v>-1.1850188616360429E-2</v>
+      </c>
+      <c r="F16" s="9">
+        <f>RANK(E16,$E$2:$E$52,1)</f>
+        <v>37</v>
+      </c>
       <c r="G16">
         <v>7352500</v>
       </c>
       <c r="H16">
         <v>7350464.0800000001</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="I16">
+        <f>H16-G16</f>
+        <v>-2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="0"/>
+        <v>-2.7697842991158804E-4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
       <c r="L16">
         <v>7397200</v>
       </c>
       <c r="M16">
         <v>7397093</v>
       </c>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>-107</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1646,23 +2146,56 @@
       <c r="C17">
         <v>14439480.050000001</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="D17">
+        <f>C17-B17</f>
+        <v>-421319.94999999925</v>
+      </c>
+      <c r="E17" s="5">
+        <f>IFERROR(D17/B17,0)</f>
+        <v>-2.8351094826658003E-2</v>
+      </c>
+      <c r="F17" s="9">
+        <f>RANK(E17,$E$2:$E$52,1)</f>
+        <v>21</v>
+      </c>
       <c r="G17">
         <v>15309700</v>
       </c>
       <c r="H17">
         <v>14645233.51</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="I17">
+        <f>H17-G17</f>
+        <v>-664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.5370836152683523E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
       <c r="L17">
         <v>15311800</v>
       </c>
       <c r="M17">
         <v>14346057.039999999</v>
       </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>-965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1672,23 +2205,56 @@
       <c r="C18">
         <v>2615303.8999999901</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="D18">
+        <f>C18-B18</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="E18" s="5">
+        <f>IFERROR(D18/B18,0)</f>
+        <v>-5.4037002206391245E-2</v>
+      </c>
+      <c r="F18" s="9">
+        <f>RANK(E18,$E$2:$E$52,1)</f>
+        <v>12</v>
+      </c>
       <c r="G18">
         <v>2861000</v>
       </c>
       <c r="H18">
         <v>2671745.94</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="I18">
+        <f>H18-G18</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.0835350460006705E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
       <c r="L18">
         <v>2910600</v>
       </c>
       <c r="M18">
         <v>2535637.09</v>
       </c>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1698,23 +2264,56 @@
       <c r="C19">
         <v>8460963.1999999899</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="D19">
+        <f>C19-B19</f>
+        <v>-376336.80000001006</v>
+      </c>
+      <c r="E19" s="5">
+        <f>IFERROR(D19/B19,0)</f>
+        <v>-4.258504294298146E-2</v>
+      </c>
+      <c r="F19" s="9">
+        <f>RANK(E19,$E$2:$E$52,1)</f>
+        <v>15</v>
+      </c>
       <c r="G19">
         <v>9713300</v>
       </c>
       <c r="H19">
         <v>8991707.2399999909</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="I19">
+        <f>H19-G19</f>
+        <v>-721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="0"/>
+        <v>-8.0250917955821899E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
       <c r="L19">
         <v>9343000</v>
       </c>
       <c r="M19">
         <v>8766655.9100000001</v>
       </c>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>-576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1724,23 +2323,56 @@
       <c r="C20">
         <v>124384360.159999</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="D20">
+        <f>C20-B20</f>
+        <v>-1539.8400010019541</v>
+      </c>
+      <c r="E20" s="5">
+        <f>IFERROR(D20/B20,0)</f>
+        <v>-1.2379538203300809E-5</v>
+      </c>
+      <c r="F20" s="9">
+        <f>RANK(E20,$E$2:$E$52,1)</f>
+        <v>46</v>
+      </c>
       <c r="G20">
         <v>131849400</v>
       </c>
       <c r="H20">
         <v>131839624.37</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="I20">
+        <f>H20-G20</f>
+        <v>-9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.4147890262190919E-5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
       <c r="L20">
         <v>130621400</v>
       </c>
       <c r="M20">
         <v>130621283.53999899</v>
       </c>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>-116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1750,23 +2382,56 @@
       <c r="C21">
         <v>22408587.5499999</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="D21">
+        <f>C21-B21</f>
+        <v>-1923512.4500000998</v>
+      </c>
+      <c r="E21" s="5">
+        <f>IFERROR(D21/B21,0)</f>
+        <v>-7.9052463618023094E-2</v>
+      </c>
+      <c r="F21" s="9">
+        <f>RANK(E21,$E$2:$E$52,1)</f>
+        <v>9</v>
+      </c>
       <c r="G21">
         <v>24497400</v>
       </c>
       <c r="H21">
         <v>22655993.629999999</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="I21">
+        <f>H21-G21</f>
+        <v>-1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="0"/>
+        <v>-8.1276787064492179E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
       <c r="L21">
         <v>24323000</v>
       </c>
       <c r="M21">
         <v>23434073.089999899</v>
       </c>
-      <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>-888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1776,23 +2441,56 @@
       <c r="C22">
         <v>11412339.8799999</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="D22">
+        <f>C22-B22</f>
+        <v>-153660.12000009976</v>
+      </c>
+      <c r="E22" s="5">
+        <f>IFERROR(D22/B22,0)</f>
+        <v>-1.3285502334437123E-2</v>
+      </c>
+      <c r="F22" s="9">
+        <f>RANK(E22,$E$2:$E$52,1)</f>
+        <v>32</v>
+      </c>
       <c r="G22">
         <v>11980700</v>
       </c>
       <c r="H22">
         <v>11791977.9699999</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="I22">
+        <f>H22-G22</f>
+        <v>-188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.6004272606362537E-2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
       <c r="L22">
         <v>11935200</v>
       </c>
       <c r="M22">
         <v>11934454.77</v>
       </c>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>-745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1802,23 +2500,56 @@
       <c r="C23">
         <v>20036743.4099999</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="D23">
+        <f>C23-B23</f>
+        <v>-825956.59000010043</v>
+      </c>
+      <c r="E23" s="5">
+        <f>IFERROR(D23/B23,0)</f>
+        <v>-3.9590110100806722E-2</v>
+      </c>
+      <c r="F23" s="9">
+        <f>RANK(E23,$E$2:$E$52,1)</f>
+        <v>18</v>
+      </c>
       <c r="G23">
         <v>22683800</v>
       </c>
       <c r="H23">
         <v>21722126.219999898</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="I23">
+        <f>H23-G23</f>
+        <v>-961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.4271622872473403E-2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="L23">
         <v>23220300</v>
       </c>
       <c r="M23">
         <v>22619057.440000001</v>
       </c>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>-601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1828,23 +2559,56 @@
       <c r="C24">
         <v>904969.19</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="D24">
+        <f>C24-B24</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="E24" s="5">
+        <f>IFERROR(D24/B24,0)</f>
+        <v>-1.3334943305713101E-2</v>
+      </c>
+      <c r="F24" s="9">
+        <f>RANK(E24,$E$2:$E$52,1)</f>
+        <v>31</v>
+      </c>
       <c r="G24">
         <v>1112700</v>
       </c>
       <c r="H24">
         <v>1067214.42</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="I24">
+        <f>H24-G24</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.2620844647132936E-2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="L24">
         <v>1112600</v>
       </c>
       <c r="M24">
         <v>1112527.1200000001</v>
       </c>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1854,23 +2618,56 @@
       <c r="C25">
         <v>479149.53</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="D25">
+        <f>C25-B25</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="E25" s="5">
+        <f>IFERROR(D25/B25,0)</f>
+        <v>-1.0226130964676661E-2</v>
+      </c>
+      <c r="F25" s="9">
+        <f>RANK(E25,$E$2:$E$52,1)</f>
+        <v>38</v>
+      </c>
       <c r="G25">
         <v>505200</v>
       </c>
       <c r="H25">
         <v>497194.20999999897</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="I25">
+        <f>H25-G25</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.6101937309368593E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
       <c r="L25">
         <v>496500</v>
       </c>
       <c r="M25">
         <v>494775.1</v>
       </c>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1880,23 +2677,56 @@
       <c r="C26">
         <v>4801960.08</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="D26">
+        <f>C26-B26</f>
+        <v>-447839.91999999993</v>
+      </c>
+      <c r="E26" s="5">
+        <f>IFERROR(D26/B26,0)</f>
+        <v>-8.5306091660634673E-2</v>
+      </c>
+      <c r="F26" s="9">
+        <f>RANK(E26,$E$2:$E$52,1)</f>
+        <v>5</v>
+      </c>
       <c r="G26">
         <v>5442200</v>
       </c>
       <c r="H26">
         <v>5122329.02999999</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="I26">
+        <f>H26-G26</f>
+        <v>-319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="0"/>
+        <v>-6.2446392671501351E-2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
       <c r="L26">
         <v>5430700</v>
       </c>
       <c r="M26">
         <v>5117235.21</v>
       </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>-313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1906,23 +2736,56 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="D27">
+        <f>C27-B27</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f>IFERROR(D27/B27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <f>RANK(E27,$E$2:$E$52,1)</f>
+        <v>47</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="I27">
+        <f>H27-G27</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1932,23 +2795,56 @@
       <c r="C28">
         <v>1250442.02</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="D28">
+        <f>C28-B28</f>
+        <v>-132457.97999999998</v>
+      </c>
+      <c r="E28" s="5">
+        <f>IFERROR(D28/B28,0)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
+      <c r="F28" s="9">
+        <f>RANK(E28,$E$2:$E$52,1)</f>
+        <v>3</v>
+      </c>
       <c r="G28">
         <v>1545700</v>
       </c>
       <c r="H28">
         <v>1281335.23</v>
       </c>
-      <c r="J28" s="5"/>
+      <c r="I28">
+        <f>H28-G28</f>
+        <v>-264364.77</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.20631975443303782</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L28">
         <v>1525900</v>
       </c>
       <c r="M28">
         <v>1393285.06</v>
       </c>
-      <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>-132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1958,23 +2854,56 @@
       <c r="C29">
         <v>2523884.71</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="D29">
+        <f>C29-B29</f>
+        <v>-37915.290000000037</v>
+      </c>
+      <c r="E29" s="5">
+        <f>IFERROR(D29/B29,0)</f>
+        <v>-1.4800253727847622E-2</v>
+      </c>
+      <c r="F29" s="9">
+        <f>RANK(E29,$E$2:$E$52,1)</f>
+        <v>28</v>
+      </c>
       <c r="G29">
         <v>2779500</v>
       </c>
       <c r="H29">
         <v>2665264.4399999902</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="I29">
+        <f>H29-G29</f>
+        <v>-114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.2860872747024777E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
       <c r="L29">
         <v>2889900</v>
       </c>
       <c r="M29">
         <v>2889864.67</v>
       </c>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>-35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1984,23 +2913,56 @@
       <c r="C30">
         <v>12030494.1</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="D30">
+        <f>C30-B30</f>
+        <v>-101705.90000000037</v>
+      </c>
+      <c r="E30" s="5">
+        <f>IFERROR(D30/B30,0)</f>
+        <v>-8.3831374359143746E-3</v>
+      </c>
+      <c r="F30" s="9">
+        <f>RANK(E30,$E$2:$E$52,1)</f>
+        <v>40</v>
+      </c>
       <c r="G30">
         <v>12735900</v>
       </c>
       <c r="H30">
         <v>12685514.279999901</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="I30">
+        <f>H30-G30</f>
+        <v>-50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.971909919295742E-3</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
       <c r="L30">
         <v>12861300</v>
       </c>
       <c r="M30">
         <v>12826009.609999999</v>
       </c>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>-35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2010,23 +2972,56 @@
       <c r="C31">
         <v>1740827.69</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="D31">
+        <f>C31-B31</f>
+        <v>-24772.310000000056</v>
+      </c>
+      <c r="E31" s="5">
+        <f>IFERROR(D31/B31,0)</f>
+        <v>-1.4030533529678329E-2</v>
+      </c>
+      <c r="F31" s="9">
+        <f>RANK(E31,$E$2:$E$52,1)</f>
+        <v>29</v>
+      </c>
       <c r="G31">
         <v>1823300</v>
       </c>
       <c r="H31">
         <v>1762676.85</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="I31">
+        <f>H31-G31</f>
+        <v>-60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.4392662500786743E-2</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
       <c r="L31">
         <v>1870700</v>
       </c>
       <c r="M31">
         <v>1801391.34</v>
       </c>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>-69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2036,23 +3031,56 @@
       <c r="C32">
         <v>5925637.7199999904</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="D32">
+        <f>C32-B32</f>
+        <v>-73762.280000009574</v>
+      </c>
+      <c r="E32" s="5">
+        <f>IFERROR(D32/B32,0)</f>
+        <v>-1.2294942827617691E-2</v>
+      </c>
+      <c r="F32" s="9">
+        <f>RANK(E32,$E$2:$E$52,1)</f>
+        <v>36</v>
+      </c>
       <c r="G32">
         <v>6195500</v>
       </c>
       <c r="H32">
         <v>6084985.4699999997</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="I32">
+        <f>H32-G32</f>
+        <v>-110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.8161839587761623E-2</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
       <c r="L32">
         <v>6157400</v>
       </c>
       <c r="M32">
         <v>5987572.0199999996</v>
       </c>
-      <c r="O32" s="5"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>-169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2062,23 +3090,56 @@
       <c r="C33">
         <v>920284264.73000002</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="D33">
+        <f>C33-B33</f>
+        <v>-7418835.2699990273</v>
+      </c>
+      <c r="E33" s="5">
+        <f>IFERROR(D33/B33,0)</f>
+        <v>-7.9969930789269058E-3</v>
+      </c>
+      <c r="F33" s="9">
+        <f>RANK(E33,$E$2:$E$52,1)</f>
+        <v>41</v>
+      </c>
       <c r="G33">
         <v>979671000</v>
       </c>
       <c r="H33">
         <v>977068513.48000002</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="I33">
+        <f>H33-G33</f>
+        <v>-2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="0"/>
+        <v>-2.6635660489465278E-3</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
       <c r="L33">
         <v>989572899.99999905</v>
       </c>
       <c r="M33">
         <v>984116289.40999901</v>
       </c>
-      <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>-5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2088,23 +3149,56 @@
       <c r="C34">
         <v>4109958.22</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="D34">
+        <f>C34-B34</f>
+        <v>-79341.779999999795</v>
+      </c>
+      <c r="E34" s="5">
+        <f>IFERROR(D34/B34,0)</f>
+        <v>-1.8939149738619768E-2</v>
+      </c>
+      <c r="F34" s="9">
+        <f>RANK(E34,$E$2:$E$52,1)</f>
+        <v>26</v>
+      </c>
       <c r="G34">
         <v>4350600</v>
       </c>
       <c r="H34">
         <v>4137588.7699999898</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="I34">
+        <f>H34-G34</f>
+        <v>-213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.1481972192227006E-2</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
       <c r="L34">
         <v>4345600</v>
       </c>
       <c r="M34">
         <v>4229801.51</v>
       </c>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>-115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2114,23 +3208,56 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="D35">
+        <f>C35-B35</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f>IFERROR(D35/B35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <f>RANK(E35,$E$2:$E$52,1)</f>
+        <v>47</v>
+      </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="I35">
+        <f>H35-G35</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="O35" s="5"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2140,23 +3267,56 @@
       <c r="C36">
         <v>735423.27999999898</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="D36">
+        <f>C36-B36</f>
+        <v>-62776.72000000102</v>
+      </c>
+      <c r="E36" s="5">
+        <f>IFERROR(D36/B36,0)</f>
+        <v>-7.8647857679780775E-2</v>
+      </c>
+      <c r="F36" s="9">
+        <f>RANK(E36,$E$2:$E$52,1)</f>
+        <v>10</v>
+      </c>
       <c r="G36">
         <v>898700</v>
       </c>
       <c r="H36">
         <v>740966.94999999902</v>
       </c>
-      <c r="J36" s="5"/>
+      <c r="I36">
+        <f>H36-G36</f>
+        <v>-157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.21287460931962104</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L36">
         <v>878300</v>
       </c>
       <c r="M36">
         <v>777215.28999999899</v>
       </c>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>-101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2166,23 +3326,56 @@
       <c r="C37">
         <v>2005447.73999999</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="D37">
+        <f>C37-B37</f>
+        <v>-82352.260000010021</v>
+      </c>
+      <c r="E37" s="5">
+        <f>IFERROR(D37/B37,0)</f>
+        <v>-3.9444515758219188E-2</v>
+      </c>
+      <c r="F37" s="9">
+        <f>RANK(E37,$E$2:$E$52,1)</f>
+        <v>19</v>
+      </c>
       <c r="G37">
         <v>2229200</v>
       </c>
       <c r="H37">
         <v>2118943.21</v>
       </c>
-      <c r="J37" s="5"/>
+      <c r="I37">
+        <f>H37-G37</f>
+        <v>-110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.2033857953182258E-2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
       <c r="L37">
         <v>2296900</v>
       </c>
       <c r="M37">
         <v>2108718.34</v>
       </c>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>-188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2192,23 +3385,56 @@
       <c r="C38">
         <v>838669.82</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="D38">
+        <f>C38-B38</f>
+        <v>-16630.180000000051</v>
+      </c>
+      <c r="E38" s="5">
+        <f>IFERROR(D38/B38,0)</f>
+        <v>-1.9443680579913542E-2</v>
+      </c>
+      <c r="F38" s="9">
+        <f>RANK(E38,$E$2:$E$52,1)</f>
+        <v>25</v>
+      </c>
       <c r="G38">
         <v>792800</v>
       </c>
       <c r="H38">
         <v>753451.96</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="I38">
+        <f>H38-G38</f>
+        <v>-39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="0"/>
+        <v>-5.2223687891129834E-2</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
       <c r="L38">
         <v>777800</v>
       </c>
       <c r="M38">
         <v>777663.26</v>
       </c>
-      <c r="O38" s="5"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>-136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2218,23 +3444,56 @@
       <c r="C39">
         <v>813108.87</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="D39">
+        <f>C39-B39</f>
+        <v>-70791.13</v>
+      </c>
+      <c r="E39" s="5">
+        <f>IFERROR(D39/B39,0)</f>
+        <v>-8.008952370177623E-2</v>
+      </c>
+      <c r="F39" s="9">
+        <f>RANK(E39,$E$2:$E$52,1)</f>
+        <v>8</v>
+      </c>
       <c r="G39">
         <v>1294400</v>
       </c>
       <c r="H39">
         <v>1114242.27999999</v>
       </c>
-      <c r="J39" s="5"/>
+      <c r="I39">
+        <f>H39-G39</f>
+        <v>-180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.16168630757756886</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="L39">
         <v>1759500</v>
       </c>
       <c r="M39">
         <v>1680463.8699999901</v>
       </c>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>-79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2244,23 +3503,56 @@
       <c r="C40">
         <v>37565141.859999903</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="D40">
+        <f>C40-B40</f>
+        <v>-816758.14000009745</v>
+      </c>
+      <c r="E40" s="5">
+        <f>IFERROR(D40/B40,0)</f>
+        <v>-2.1279773539092578E-2</v>
+      </c>
+      <c r="F40" s="9">
+        <f>RANK(E40,$E$2:$E$52,1)</f>
+        <v>23</v>
+      </c>
       <c r="G40">
         <v>39964900</v>
       </c>
       <c r="H40">
         <v>38095240.189999901</v>
       </c>
-      <c r="J40" s="5"/>
+      <c r="I40">
+        <f>H40-G40</f>
+        <v>-1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.9078567313795014E-2</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
       <c r="L40">
         <v>40216700</v>
       </c>
       <c r="M40">
         <v>39606263.709999897</v>
       </c>
-      <c r="O40" s="5"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>-610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2270,23 +3562,56 @@
       <c r="C41">
         <v>4409060.2099999897</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="D41">
+        <f>C41-B41</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="E41" s="5">
+        <f>IFERROR(D41/B41,0)</f>
+        <v>-4.0110550149132493E-2</v>
+      </c>
+      <c r="F41" s="9">
+        <f>RANK(E41,$E$2:$E$52,1)</f>
+        <v>17</v>
+      </c>
       <c r="G41">
         <v>5089500</v>
       </c>
       <c r="H41">
         <v>4956043.6699999897</v>
       </c>
-      <c r="J41" s="5"/>
+      <c r="I41">
+        <f>H41-G41</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="0"/>
+        <v>-2.6927997186112485E-2</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
       <c r="L41">
         <v>4799900</v>
       </c>
       <c r="M41">
         <v>4717822.6500000004</v>
       </c>
-      <c r="O41" s="5"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2296,23 +3621,56 @@
       <c r="C42">
         <v>188551675.67999899</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="D42">
+        <f>C42-B42</f>
+        <v>-41624.320001006126</v>
+      </c>
+      <c r="E42" s="5">
+        <f>IFERROR(D42/B42,0)</f>
+        <v>-2.2070943135841053E-4</v>
+      </c>
+      <c r="F42" s="9">
+        <f>RANK(E42,$E$2:$E$52,1)</f>
+        <v>44</v>
+      </c>
       <c r="G42">
         <v>199130300</v>
       </c>
       <c r="H42">
         <v>196755033.31</v>
       </c>
-      <c r="J42" s="5"/>
+      <c r="I42">
+        <f>H42-G42</f>
+        <v>-2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.2072202931945403E-2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
       <c r="L42">
         <v>199954600</v>
       </c>
       <c r="M42">
         <v>199954563.74999899</v>
       </c>
-      <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>-36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2322,23 +3680,56 @@
       <c r="C43">
         <v>7968645.8300000001</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="D43">
+        <f>C43-B43</f>
+        <v>-166754.16999999993</v>
+      </c>
+      <c r="E43" s="5">
+        <f>IFERROR(D43/B43,0)</f>
+        <v>-2.0497353541313264E-2</v>
+      </c>
+      <c r="F43" s="9">
+        <f>RANK(E43,$E$2:$E$52,1)</f>
+        <v>24</v>
+      </c>
       <c r="G43">
         <v>8560800</v>
       </c>
       <c r="H43">
         <v>8171472.0199999996</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="I43">
+        <f>H43-G43</f>
+        <v>-389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.764477918386123E-2</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
       <c r="L43">
         <v>8497500</v>
       </c>
       <c r="M43">
         <v>8150982.5699999901</v>
       </c>
-      <c r="O43" s="5"/>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>-346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2348,23 +3739,56 @@
       <c r="C44">
         <v>29789104.379999999</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="D44">
+        <f>C44-B44</f>
+        <v>-294095.62000000104</v>
+      </c>
+      <c r="E44" s="5">
+        <f>IFERROR(D44/B44,0)</f>
+        <v>-9.7760750186150751E-3</v>
+      </c>
+      <c r="F44" s="9">
+        <f>RANK(E44,$E$2:$E$52,1)</f>
+        <v>39</v>
+      </c>
       <c r="G44">
         <v>31040700</v>
       </c>
       <c r="H44">
         <v>30793711.48</v>
       </c>
-      <c r="J44" s="5"/>
+      <c r="I44">
+        <f>H44-G44</f>
+        <v>-246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" si="0"/>
+        <v>-8.0207454096728314E-3</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
       <c r="L44">
         <v>31282200</v>
       </c>
       <c r="M44">
         <v>31282141.25</v>
       </c>
-      <c r="O44" s="5"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>-58.75</v>
+      </c>
+      <c r="O44" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2374,23 +3798,56 @@
       <c r="C45">
         <v>54589584.0499999</v>
       </c>
-      <c r="E45" s="5"/>
+      <c r="D45">
+        <f>C45-B45</f>
+        <v>-712015.95000009984</v>
+      </c>
+      <c r="E45" s="5">
+        <f>IFERROR(D45/B45,0)</f>
+        <v>-1.287514194887851E-2</v>
+      </c>
+      <c r="F45" s="9">
+        <f>RANK(E45,$E$2:$E$52,1)</f>
+        <v>34</v>
+      </c>
       <c r="G45">
         <v>56792200</v>
       </c>
       <c r="H45">
         <v>54594953.959999897</v>
       </c>
-      <c r="J45" s="5"/>
+      <c r="I45">
+        <f>H45-G45</f>
+        <v>-2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.0246320962372462E-2</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
       <c r="L45">
         <v>56027100</v>
       </c>
       <c r="M45">
         <v>55386549.6599999</v>
       </c>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>-640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2400,23 +3857,56 @@
       <c r="C46">
         <v>258322.43</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="D46">
+        <f>C46-B46</f>
+        <v>-777.57000000000698</v>
+      </c>
+      <c r="E46" s="5">
+        <f>IFERROR(D46/B46,0)</f>
+        <v>-3.0010420686993711E-3</v>
+      </c>
+      <c r="F46" s="9">
+        <f>RANK(E46,$E$2:$E$52,1)</f>
+        <v>43</v>
+      </c>
       <c r="G46">
         <v>266000</v>
       </c>
       <c r="H46">
         <v>257402.90999999901</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="I46">
+        <f>H46-G46</f>
+        <v>-8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.3399350458007716E-2</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
       <c r="L46">
         <v>267100</v>
       </c>
       <c r="M46">
         <v>254753.15999999901</v>
       </c>
-      <c r="O46" s="5"/>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>-12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2426,23 +3916,56 @@
       <c r="C47">
         <v>70378426.719999999</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="D47">
+        <f>C47-B47</f>
+        <v>-12273.280000001192</v>
+      </c>
+      <c r="E47" s="5">
+        <f>IFERROR(D47/B47,0)</f>
+        <v>-1.7435939690898361E-4</v>
+      </c>
+      <c r="F47" s="9">
+        <f>RANK(E47,$E$2:$E$52,1)</f>
+        <v>45</v>
+      </c>
       <c r="G47">
         <v>73467000</v>
       </c>
       <c r="H47">
         <v>73442541.659999996</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="I47">
+        <f>H47-G47</f>
+        <v>-24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.330268730789944E-4</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
       <c r="L47">
         <v>75072800</v>
       </c>
       <c r="M47">
         <v>75050829.179999903</v>
       </c>
-      <c r="O47" s="5"/>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>-21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2452,23 +3975,56 @@
       <c r="C48">
         <v>6527352.5699999901</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="D48">
+        <f>C48-B48</f>
+        <v>-209747.43000000995</v>
+      </c>
+      <c r="E48" s="5">
+        <f>IFERROR(D48/B48,0)</f>
+        <v>-3.1133192323107857E-2</v>
+      </c>
+      <c r="F48" s="9">
+        <f>RANK(E48,$E$2:$E$52,1)</f>
+        <v>20</v>
+      </c>
       <c r="G48">
         <v>7214700</v>
       </c>
       <c r="H48">
         <v>6922072.5599999996</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="I48">
+        <f>H48-G48</f>
+        <v>-292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.2274540964939038E-2</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
       <c r="L48">
         <v>7289800</v>
       </c>
       <c r="M48">
         <v>6882350.23999999</v>
       </c>
-      <c r="O48" s="5"/>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>-407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2478,23 +4034,56 @@
       <c r="C49">
         <v>90499.43</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="D49">
+        <f>C49-B49</f>
+        <v>-1700.570000000007</v>
+      </c>
+      <c r="E49" s="5">
+        <f>IFERROR(D49/B49,0)</f>
+        <v>-1.8444360086767971E-2</v>
+      </c>
+      <c r="F49" s="9">
+        <f>RANK(E49,$E$2:$E$52,1)</f>
+        <v>27</v>
+      </c>
       <c r="G49">
         <v>102600</v>
       </c>
       <c r="H49">
         <v>95466.880000000005</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="I49">
+        <f>H49-G49</f>
+        <v>-7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.4718268785991485E-2</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="O49" s="5"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2504,23 +4093,56 @@
       <c r="C50">
         <v>832600</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="D50">
+        <f>C50-B50</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <f>IFERROR(D50/B50,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="9">
+        <f>RANK(E50,$E$2:$E$52,1)</f>
+        <v>47</v>
+      </c>
       <c r="G50">
         <v>859100</v>
       </c>
       <c r="H50">
         <v>859100</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="I50">
+        <f>H50-G50</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
       <c r="L50">
         <v>843200</v>
       </c>
       <c r="M50">
         <v>843200</v>
       </c>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2530,23 +4152,56 @@
       <c r="C51">
         <v>8499425.3399999905</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="D51">
+        <f>C51-B51</f>
+        <v>-110074.66000000946</v>
+      </c>
+      <c r="E51" s="5">
+        <f>IFERROR(D51/B51,0)</f>
+        <v>-1.2785255822058129E-2</v>
+      </c>
+      <c r="F51" s="9">
+        <f>RANK(E51,$E$2:$E$52,1)</f>
+        <v>35</v>
+      </c>
       <c r="G51">
         <v>8925500</v>
       </c>
       <c r="H51">
         <v>8599059.6199999992</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="I51">
+        <f>H51-G51</f>
+        <v>-326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.796233476981066E-2</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
       <c r="L51">
         <v>8833900</v>
       </c>
       <c r="M51">
         <v>8735843.3100000005</v>
       </c>
-      <c r="O51" s="5"/>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>-98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2556,28 +4211,61 @@
       <c r="C52">
         <v>2254684.7999999998</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="D52">
+        <f>C52-B52</f>
+        <v>-196315.20000000019</v>
+      </c>
+      <c r="E52" s="5">
+        <f>IFERROR(D52/B52,0)</f>
+        <v>-8.009596083231342E-2</v>
+      </c>
+      <c r="F52" s="9">
+        <f>RANK(E52,$E$2:$E$52,1)</f>
+        <v>7</v>
+      </c>
       <c r="G52">
         <v>2440700</v>
       </c>
       <c r="H52">
         <v>2204672.88</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="I52">
+        <f>H52-G52</f>
+        <v>-236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.10705766018222174</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="L52">
         <v>2321600</v>
       </c>
       <c r="M52">
         <v>2056835.26</v>
       </c>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="54" spans="1:15" ht="15">
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>-264764.74</v>
+      </c>
+      <c r="O52" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,42 +4279,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="B56">
+        <f>VLOOKUP(A56,$A$2:$P$52,4,FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56,$A$2:$P$52,9,FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP(A56,$A$2:$P$52,14,FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="B57">
+        <f t="shared" ref="B57:B61" si="5">VLOOKUP(A57,$A$2:$P$52,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57:C61" si="6">VLOOKUP(A57,$A$2:$P$52,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57:D61" si="7">VLOOKUP(A57,$A$2:$P$52,14,FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="B58">
+        <f t="shared" si="5"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="6"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="7"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="B59">
+        <f t="shared" si="5"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="6"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="7"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="B60">
+        <f t="shared" si="5"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="6"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="7"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="15">
+      <c r="B61">
+        <f t="shared" si="5"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="6"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="7"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2640,43 +4400,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15">
+      <c r="B65">
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$D$2:$D$52)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C65">
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15">
+      <c r="B66">
+        <f t="shared" ref="B66:B70" si="8">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C70" si="9">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D70" si="10">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="B67">
+        <f t="shared" si="8"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="9"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="10"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="B68">
+        <f t="shared" si="8"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="9"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="10"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="B69">
+        <f t="shared" si="8"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="9"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="10"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15"/>
-    <row r="72" spans="1:4" ht="15">
+      <c r="B70">
+        <f t="shared" si="8"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="9"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="10"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2690,48 +4521,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15">
+      <c r="B74">
+        <f>INDEX($D$2:$D$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX($I$2:$I$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="11">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C79" si="12">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D79" si="13">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="B76">
+        <f t="shared" si="11"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="12"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="13"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="B77">
+        <f t="shared" si="11"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="12"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="13"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="B78">
+        <f t="shared" si="11"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="12"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="13"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15"/>
-    <row r="81" spans="1:7" ht="15">
+      <c r="B79">
+        <f t="shared" si="11"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="12"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="13"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -2739,50 +4641,76 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="B84" s="6">
+        <f>IFERROR(INDEX($B$2:$B$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>356640100</v>
+      </c>
+      <c r="C84" s="6">
+        <f>IFERROR(INDEX($C$2:$C$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>341243679.13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="B85" s="6">
+        <f>IFERROR(INDEX($G$2:$G$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>382685200</v>
+      </c>
+      <c r="C85" s="6">
+        <f>IFERROR(INDEX($H$2:$H$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>346340810.81999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-    </row>
-    <row r="87" spans="1:7" ht="15"/>
-    <row r="88" spans="1:7" ht="15">
+      <c r="B86" s="6">
+        <f>IFERROR(INDEX($L$2:$L$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>376548600</v>
+      </c>
+      <c r="C86" s="6">
+        <f>IFERROR(INDEX($M$2:$M$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
+        <v>355279492.22999901</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15">
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>77</v>
       </c>
       <c r="B89" s="7">
         <v>1</v>
       </c>
-      <c r="C89" s="7"/>
+      <c r="C89" s="6"/>
       <c r="D89" s="7">
         <v>2</v>
       </c>
       <c r="E89" s="7"/>
-      <c r="F89" s="7">
+      <c r="F89" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -2795,14 +4723,14 @@
       <c r="E90" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="F90" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G90" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +4738,7 @@
       <c r="E91" s="5"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -2818,7 +4746,7 @@
       <c r="E92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -2826,12 +4754,12 @@
       <c r="E93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="15">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -2843,11 +4771,11 @@
         <v>2</v>
       </c>
       <c r="E96" s="7"/>
-      <c r="F96" s="7">
+      <c r="F96" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B97" s="8" t="s">
         <v>0</v>
       </c>
@@ -2860,14 +4788,14 @@
       <c r="E97" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F97" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2876,7 +4804,7 @@
       <c r="G98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -2885,7 +4813,7 @@
       <c r="G99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -2894,15 +4822,12 @@
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="102" spans="1:9" ht="15"/>
-    <row r="103" spans="1:9" ht="15"/>
-    <row r="104" spans="1:9" ht="15"/>
-    <row r="105" spans="1:9" ht="15"/>
-    <row r="106" spans="1:9" ht="15"/>
-    <row r="107" spans="1:9" ht="15"/>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F52">
+    <sortCondition ref="F2:F52"/>
+  </sortState>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 A87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
@@ -2919,13 +4844,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +4858,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +4866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2949,7 +4874,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +4882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2965,7 +4890,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +4898,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2981,7 +4906,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +4914,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2997,7 +4922,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Lookup exercise Sept 19 push 7:18 pm
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\Documents\NSS-DA13\Excel\lookups-exercise-RenukaD13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B674FEA7-32CF-479B-83A7-589E48A727F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD8B44A-EDB5-4FBF-8008-3119B2E87921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,13 @@
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">metro_budget!$A$84:$A$87</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">metro_budget!$B$83</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">metro_budget!$B$84:$B$87</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">metro_budget!$C$83</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">metro_budget!$C$84:$C$87</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +333,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Diffrence</t>
   </si>
 </sst>
 </file>
@@ -809,7 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,11 +851,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -882,6 +909,1127 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Administrative Budget and Actual amount for fiscal years. </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assessor of Property</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$87</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7670700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7968300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7759600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2879-4F1A-8306-52031C22A6E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assessor of Property</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$87</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6947552.6699999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7020609.3200000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7497322.9100000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2879-4F1A-8306-52031C22A6E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="873138287"/>
+        <c:axId val="873124847"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$D$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diffrence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Assessor of Property</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$D$84:$D$87</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-723147.33000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-947690.6799999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-262277.08999999985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2879-4F1A-8306-52031C22A6E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="873138287"/>
+        <c:axId val="873124847"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="873138287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873124847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="873124847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873138287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1044575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>11112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>36512</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E6B75C-C8C2-90FF-53AA-F71797AFDAC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1192,7 +2340,7 @@
     <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.54296875" customWidth="1"/>
     <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.81640625" customWidth="1"/>
@@ -1217,7 +2365,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1262,15 +2410,15 @@
         <v>341243679.13</v>
       </c>
       <c r="D2">
-        <f>C2-B2</f>
+        <f t="shared" ref="D2:D33" si="0">C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
         <f>IFERROR(D2/B2,0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2" s="9">
-        <f>RANK(E2,$E$2:$E$52,1)</f>
+      <c r="F2">
+        <f>_xlfn.RANK.EQ(E2,$E$2:$E$52,1)</f>
         <v>14</v>
       </c>
       <c r="G2">
@@ -1280,7 +2428,7 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f>H2-G2</f>
+        <f t="shared" ref="I2:I33" si="1">H2-G2</f>
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
@@ -1288,7 +2436,7 @@
         <v>-0.10493822282725118</v>
       </c>
       <c r="K2">
-        <f>RANK(J2,$J$2:$J$52,1)</f>
+        <f>_xlfn.RANK.EQ(J2,$J$2:$J$52,1)</f>
         <v>10</v>
       </c>
       <c r="L2">
@@ -1306,7 +2454,7 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>RANK(O2,$O$2:$O$52,1)</f>
+        <f>_xlfn.RANK.EQ(O2,$O$2:$O$52,1)</f>
         <v>14</v>
       </c>
     </row>
@@ -1325,11 +2473,11 @@
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f>IFERROR(D3/B3,0)</f>
+        <f t="shared" ref="E3:E33" si="2">IFERROR(D3/B3,0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3" s="9">
-        <f>RANK(E3,$E$2:$E$52,1)</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F52" si="3">_xlfn.RANK.EQ(E3,$E$2:$E$52,1)</f>
         <v>22</v>
       </c>
       <c r="G3">
@@ -1339,15 +2487,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f>H3-G3</f>
+        <f t="shared" si="1"/>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="0">IFERROR(I3/H3,0)</f>
+        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/H3,0)</f>
         <v>-7.1587313673678488E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="1">RANK(J3,$J$2:$J$52,1)</f>
+        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3,$J$2:$J$52,1)</f>
         <v>14</v>
       </c>
       <c r="L3">
@@ -1357,15 +2505,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="2">M3-L3</f>
+        <f t="shared" ref="N3:N52" si="6">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="3">IFERROR(N3/L3,0)</f>
+        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="4">RANK(O3,$O$2:$O$52,1)</f>
+        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3,$O$2:$O$52,1)</f>
         <v>37</v>
       </c>
     </row>
@@ -1380,15 +2528,15 @@
         <v>3115157.5599999898</v>
       </c>
       <c r="D4">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
-        <f>IFERROR(D4/B4,0)</f>
+        <f t="shared" si="2"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4" s="9">
-        <f>RANK(E4,$E$2:$E$52,1)</f>
+      <c r="F4">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="G4">
@@ -1398,15 +2546,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
-        <f>H4-G4</f>
+        <f t="shared" si="1"/>
         <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.7440707697694863E-2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L4">
@@ -1416,15 +2564,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
     </row>
@@ -1439,15 +2587,15 @@
         <v>6947552.6699999999</v>
       </c>
       <c r="D5">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
-        <f>IFERROR(D5/B5,0)</f>
+        <f t="shared" si="2"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5" s="9">
-        <f>RANK(E5,$E$2:$E$52,1)</f>
+      <c r="F5">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G5">
@@ -1457,15 +2605,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
-        <f>H5-G5</f>
+        <f t="shared" si="1"/>
         <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.13498695580457107</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L5">
@@ -1475,15 +2623,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
     </row>
@@ -1498,15 +2646,15 @@
         <v>385908.52</v>
       </c>
       <c r="D6">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
-        <f>IFERROR(D6/B6,0)</f>
+        <f t="shared" si="2"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6" s="9">
-        <f>RANK(E6,$E$2:$E$52,1)</f>
+      <c r="F6">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G6">
@@ -1516,15 +2664,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
-        <f>H6-G6</f>
+        <f t="shared" si="1"/>
         <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.7331268866947632E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="L6">
@@ -1534,15 +2682,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
     </row>
@@ -1557,15 +2705,15 @@
         <v>2946071.21</v>
       </c>
       <c r="D7">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
-        <f>IFERROR(D7/B7,0)</f>
+        <f t="shared" si="2"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7" s="9">
-        <f>RANK(E7,$E$2:$E$52,1)</f>
+      <c r="F7">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G7">
@@ -1575,15 +2723,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
-        <f>H7-G7</f>
+        <f t="shared" si="1"/>
         <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.11123002959403271</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L7">
@@ -1593,15 +2741,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -1616,15 +2764,15 @@
         <v>1315623.30999999</v>
       </c>
       <c r="D8">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
-        <f>IFERROR(D8/B8,0)</f>
+        <f t="shared" si="2"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8" s="9">
-        <f>RANK(E8,$E$2:$E$52,1)</f>
+      <c r="F8">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1634,15 +2782,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
-        <f>H8-G8</f>
+        <f t="shared" si="1"/>
         <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.14942778736004425</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L8">
@@ -1652,15 +2800,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -1675,15 +2823,15 @@
         <v>8952825.2799999993</v>
       </c>
       <c r="D9">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
-        <f>IFERROR(D9/B9,0)</f>
+        <f t="shared" si="2"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9" s="9">
-        <f>RANK(E9,$E$2:$E$52,1)</f>
+      <c r="F9">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G9">
@@ -1693,15 +2841,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
-        <f>H9-G9</f>
+        <f t="shared" si="1"/>
         <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.11528186307014912</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L9">
@@ -1711,15 +2859,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -1734,15 +2882,15 @@
         <v>407090.37</v>
       </c>
       <c r="D10">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
-        <f>IFERROR(D10/B10,0)</f>
+        <f t="shared" si="2"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10" s="9">
-        <f>RANK(E10,$E$2:$E$52,1)</f>
+      <c r="F10">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G10">
@@ -1752,15 +2900,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
-        <f>H10-G10</f>
+        <f t="shared" si="1"/>
         <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5.8328067339072524E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="L10">
@@ -1770,15 +2918,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
     </row>
@@ -1793,15 +2941,15 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="5">
-        <f>IFERROR(D11/B11,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="9">
-        <f>RANK(E11,$E$2:$E$52,1)</f>
+      <c r="F11">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G11">
@@ -1811,15 +2959,15 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>H11-G11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L11">
@@ -1829,15 +2977,15 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -1852,15 +3000,15 @@
         <v>4066595.33</v>
       </c>
       <c r="D12">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
-        <f>IFERROR(D12/B12,0)</f>
+        <f t="shared" si="2"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12" s="9">
-        <f>RANK(E12,$E$2:$E$52,1)</f>
+      <c r="F12">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="G12">
@@ -1870,15 +3018,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
-        <f>H12-G12</f>
+        <f t="shared" si="1"/>
         <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.11766445318188171</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L12">
@@ -1888,15 +3036,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -1911,15 +3059,15 @@
         <v>5772288.3300000001</v>
       </c>
       <c r="D13">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
-        <f>IFERROR(D13/B13,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13" s="9">
-        <f>RANK(E13,$E$2:$E$52,1)</f>
+      <c r="F13">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="G13">
@@ -1929,15 +3077,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
-        <f>H13-G13</f>
+        <f t="shared" si="1"/>
         <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5.3243850088734883E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="L13">
@@ -1947,15 +3095,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
     </row>
@@ -1970,15 +3118,15 @@
         <v>505017.37</v>
       </c>
       <c r="D14">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
-        <f>IFERROR(D14/B14,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14" s="9">
-        <f>RANK(E14,$E$2:$E$52,1)</f>
+      <c r="F14">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="G14">
@@ -1988,15 +3136,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
-        <f>H14-G14</f>
+        <f t="shared" si="1"/>
         <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.1626592968636483E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="L14">
@@ -2006,15 +3154,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
     </row>
@@ -2029,15 +3177,15 @@
         <v>156545919.90000001</v>
       </c>
       <c r="D15">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
-        <f>IFERROR(D15/B15,0)</f>
+        <f t="shared" si="2"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15" s="9">
-        <f>RANK(E15,$E$2:$E$52,1)</f>
+      <c r="F15">
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="G15">
@@ -2047,15 +3195,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
-        <f>H15-G15</f>
+        <f t="shared" si="1"/>
         <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.6607825420280143E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L15">
@@ -2065,15 +3213,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
     </row>
@@ -2088,15 +3236,15 @@
         <v>6522480.4599999897</v>
       </c>
       <c r="D16">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
-        <f>IFERROR(D16/B16,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16" s="9">
-        <f>RANK(E16,$E$2:$E$52,1)</f>
+      <c r="F16">
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="G16">
@@ -2106,15 +3254,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
-        <f>H16-G16</f>
+        <f t="shared" si="1"/>
         <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-2.7697842991158804E-4</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="L16">
@@ -2124,15 +3272,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>43</v>
       </c>
     </row>
@@ -2147,15 +3295,15 @@
         <v>14439480.050000001</v>
       </c>
       <c r="D17">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
-        <f>IFERROR(D17/B17,0)</f>
+        <f t="shared" si="2"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17" s="9">
-        <f>RANK(E17,$E$2:$E$52,1)</f>
+      <c r="F17">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="G17">
@@ -2165,15 +3313,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
-        <f>H17-G17</f>
+        <f t="shared" si="1"/>
         <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.5370836152683523E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="L17">
@@ -2183,15 +3331,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -2206,15 +3354,15 @@
         <v>2615303.8999999901</v>
       </c>
       <c r="D18">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
-        <f>IFERROR(D18/B18,0)</f>
+        <f t="shared" si="2"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18" s="9">
-        <f>RANK(E18,$E$2:$E$52,1)</f>
+      <c r="F18">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G18">
@@ -2224,15 +3372,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
-        <f>H18-G18</f>
+        <f t="shared" si="1"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-7.0835350460006705E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="L18">
@@ -2242,15 +3390,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -2265,15 +3413,15 @@
         <v>8460963.1999999899</v>
       </c>
       <c r="D19">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
-        <f>IFERROR(D19/B19,0)</f>
+        <f t="shared" si="2"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19" s="9">
-        <f>RANK(E19,$E$2:$E$52,1)</f>
+      <c r="F19">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="G19">
@@ -2283,15 +3431,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
-        <f>H19-G19</f>
+        <f t="shared" si="1"/>
         <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-8.0250917955821899E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="L19">
@@ -2301,15 +3449,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -2324,15 +3472,15 @@
         <v>124384360.159999</v>
       </c>
       <c r="D20">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f>IFERROR(D20/B20,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20" s="9">
-        <f>RANK(E20,$E$2:$E$52,1)</f>
+      <c r="F20">
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="G20">
@@ -2342,15 +3490,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
-        <f>H20-G20</f>
+        <f t="shared" si="1"/>
         <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-7.4147890262190919E-5</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="L20">
@@ -2360,15 +3508,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
     </row>
@@ -2383,15 +3531,15 @@
         <v>22408587.5499999</v>
       </c>
       <c r="D21">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
-        <f>IFERROR(D21/B21,0)</f>
+        <f t="shared" si="2"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21" s="9">
-        <f>RANK(E21,$E$2:$E$52,1)</f>
+      <c r="F21">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G21">
@@ -2401,15 +3549,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
-        <f>H21-G21</f>
+        <f t="shared" si="1"/>
         <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-8.1276787064492179E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="L21">
@@ -2419,15 +3567,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -2442,15 +3590,15 @@
         <v>11412339.8799999</v>
       </c>
       <c r="D22">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
-        <f>IFERROR(D22/B22,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22" s="9">
-        <f>RANK(E22,$E$2:$E$52,1)</f>
+      <c r="F22">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="G22">
@@ -2460,15 +3608,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
-        <f>H22-G22</f>
+        <f t="shared" si="1"/>
         <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.6004272606362537E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="L22">
@@ -2478,15 +3626,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
     </row>
@@ -2501,15 +3649,15 @@
         <v>20036743.4099999</v>
       </c>
       <c r="D23">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
-        <f>IFERROR(D23/B23,0)</f>
+        <f t="shared" si="2"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23" s="9">
-        <f>RANK(E23,$E$2:$E$52,1)</f>
+      <c r="F23">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G23">
@@ -2519,15 +3667,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
-        <f>H23-G23</f>
+        <f t="shared" si="1"/>
         <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.4271622872473403E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="L23">
@@ -2537,15 +3685,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
     </row>
@@ -2560,15 +3708,15 @@
         <v>904969.19</v>
       </c>
       <c r="D24">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
-        <f>IFERROR(D24/B24,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24" s="9">
-        <f>RANK(E24,$E$2:$E$52,1)</f>
+      <c r="F24">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="G24">
@@ -2578,15 +3726,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
-        <f>H24-G24</f>
+        <f t="shared" si="1"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.2620844647132936E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="L24">
@@ -2596,15 +3744,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
     </row>
@@ -2619,15 +3767,15 @@
         <v>479149.53</v>
       </c>
       <c r="D25">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
-        <f>IFERROR(D25/B25,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25" s="9">
-        <f>RANK(E25,$E$2:$E$52,1)</f>
+      <c r="F25">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="G25">
@@ -2637,15 +3785,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
-        <f>H25-G25</f>
+        <f t="shared" si="1"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.6101937309368593E-2</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="L25">
@@ -2655,15 +3803,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
     </row>
@@ -2678,15 +3826,15 @@
         <v>4801960.08</v>
       </c>
       <c r="D26">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
-        <f>IFERROR(D26/B26,0)</f>
+        <f t="shared" si="2"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26" s="9">
-        <f>RANK(E26,$E$2:$E$52,1)</f>
+      <c r="F26">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G26">
@@ -2696,15 +3844,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
-        <f>H26-G26</f>
+        <f t="shared" si="1"/>
         <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-6.2446392671501351E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="L26">
@@ -2714,15 +3862,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
     </row>
@@ -2737,15 +3885,15 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f>C27-B27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="5">
-        <f>IFERROR(D27/B27,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27" s="9">
-        <f>RANK(E27,$E$2:$E$52,1)</f>
+      <c r="F27">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G27">
@@ -2755,15 +3903,15 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>H27-G27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J27" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L27">
@@ -2773,15 +3921,15 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -2796,15 +3944,15 @@
         <v>1250442.02</v>
       </c>
       <c r="D28">
-        <f>C28-B28</f>
+        <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
-        <f>IFERROR(D28/B28,0)</f>
+        <f t="shared" si="2"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28" s="9">
-        <f>RANK(E28,$E$2:$E$52,1)</f>
+      <c r="F28">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G28">
@@ -2814,15 +3962,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
-        <f>H28-G28</f>
+        <f t="shared" si="1"/>
         <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.20631975443303782</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L28">
@@ -2832,15 +3980,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -2855,15 +4003,15 @@
         <v>2523884.71</v>
       </c>
       <c r="D29">
-        <f>C29-B29</f>
+        <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
-        <f>IFERROR(D29/B29,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29" s="9">
-        <f>RANK(E29,$E$2:$E$52,1)</f>
+      <c r="F29">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="G29">
@@ -2873,15 +4021,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
-        <f>H29-G29</f>
+        <f t="shared" si="1"/>
         <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.2860872747024777E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="L29">
@@ -2891,15 +4039,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
     </row>
@@ -2914,15 +4062,15 @@
         <v>12030494.1</v>
       </c>
       <c r="D30">
-        <f>C30-B30</f>
+        <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
-        <f>IFERROR(D30/B30,0)</f>
+        <f t="shared" si="2"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30" s="9">
-        <f>RANK(E30,$E$2:$E$52,1)</f>
+      <c r="F30">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G30">
@@ -2932,15 +4080,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
-        <f>H30-G30</f>
+        <f t="shared" si="1"/>
         <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-3.971909919295742E-3</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="L30">
@@ -2950,15 +4098,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
     </row>
@@ -2973,15 +4121,15 @@
         <v>1740827.69</v>
       </c>
       <c r="D31">
-        <f>C31-B31</f>
+        <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
-        <f>IFERROR(D31/B31,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31" s="9">
-        <f>RANK(E31,$E$2:$E$52,1)</f>
+      <c r="F31">
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="G31">
@@ -2991,15 +4139,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
-        <f>H31-G31</f>
+        <f t="shared" si="1"/>
         <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-3.4392662500786743E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="L31">
@@ -3009,15 +4157,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
@@ -3032,15 +4180,15 @@
         <v>5925637.7199999904</v>
       </c>
       <c r="D32">
-        <f>C32-B32</f>
+        <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
-        <f>IFERROR(D32/B32,0)</f>
+        <f t="shared" si="2"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32" s="9">
-        <f>RANK(E32,$E$2:$E$52,1)</f>
+      <c r="F32">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="G32">
@@ -3050,15 +4198,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
-        <f>H32-G32</f>
+        <f t="shared" si="1"/>
         <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.8161839587761623E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="L32">
@@ -3068,15 +4216,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
     </row>
@@ -3091,15 +4239,15 @@
         <v>920284264.73000002</v>
       </c>
       <c r="D33">
-        <f>C33-B33</f>
+        <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
-        <f>IFERROR(D33/B33,0)</f>
+        <f t="shared" si="2"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33" s="9">
-        <f>RANK(E33,$E$2:$E$52,1)</f>
+      <c r="F33">
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="G33">
@@ -3109,15 +4257,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
-        <f>H33-G33</f>
+        <f t="shared" si="1"/>
         <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-2.6635660489465278E-3</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="L33">
@@ -3127,15 +4275,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
     </row>
@@ -3150,15 +4298,15 @@
         <v>4109958.22</v>
       </c>
       <c r="D34">
-        <f>C34-B34</f>
+        <f t="shared" ref="D34:D52" si="9">C34-B34</f>
         <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
-        <f>IFERROR(D34/B34,0)</f>
+        <f t="shared" ref="E34:E52" si="10">IFERROR(D34/B34,0)</f>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34" s="9">
-        <f>RANK(E34,$E$2:$E$52,1)</f>
+      <c r="F34">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="G34">
@@ -3168,15 +4316,15 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
-        <f>H34-G34</f>
+        <f t="shared" ref="I34:I52" si="11">H34-G34</f>
         <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5.1481972192227006E-2</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="L34">
@@ -3186,15 +4334,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
     </row>
@@ -3209,15 +4357,15 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f>C35-B35</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E35" s="5">
-        <f>IFERROR(D35/B35,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F35" s="9">
-        <f>RANK(E35,$E$2:$E$52,1)</f>
+      <c r="F35">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G35">
@@ -3227,15 +4375,15 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <f>H35-G35</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L35">
@@ -3245,15 +4393,15 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -3268,15 +4416,15 @@
         <v>735423.27999999898</v>
       </c>
       <c r="D36">
-        <f>C36-B36</f>
+        <f t="shared" si="9"/>
         <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
-        <f>IFERROR(D36/B36,0)</f>
+        <f t="shared" si="10"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36" s="9">
-        <f>RANK(E36,$E$2:$E$52,1)</f>
+      <c r="F36">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G36">
@@ -3286,15 +4434,15 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
-        <f>H36-G36</f>
+        <f t="shared" si="11"/>
         <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.21287460931962104</v>
       </c>
       <c r="K36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L36">
@@ -3304,15 +4452,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -3327,15 +4475,15 @@
         <v>2005447.73999999</v>
       </c>
       <c r="D37">
-        <f>C37-B37</f>
+        <f t="shared" si="9"/>
         <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
-        <f>IFERROR(D37/B37,0)</f>
+        <f t="shared" si="10"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37" s="9">
-        <f>RANK(E37,$E$2:$E$52,1)</f>
+      <c r="F37">
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="G37">
@@ -3345,15 +4493,15 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
-        <f>H37-G37</f>
+        <f t="shared" si="11"/>
         <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5.2033857953182258E-2</v>
       </c>
       <c r="K37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="L37">
@@ -3363,15 +4511,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -3386,15 +4534,15 @@
         <v>838669.82</v>
       </c>
       <c r="D38">
-        <f>C38-B38</f>
+        <f t="shared" si="9"/>
         <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
-        <f>IFERROR(D38/B38,0)</f>
+        <f t="shared" si="10"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38" s="9">
-        <f>RANK(E38,$E$2:$E$52,1)</f>
+      <c r="F38">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G38">
@@ -3404,15 +4552,15 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
-        <f>H38-G38</f>
+        <f t="shared" si="11"/>
         <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-5.2223687891129834E-2</v>
       </c>
       <c r="K38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="L38">
@@ -3422,15 +4570,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
     </row>
@@ -3445,15 +4593,15 @@
         <v>813108.87</v>
       </c>
       <c r="D39">
-        <f>C39-B39</f>
+        <f t="shared" si="9"/>
         <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
-        <f>IFERROR(D39/B39,0)</f>
+        <f t="shared" si="10"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39" s="9">
-        <f>RANK(E39,$E$2:$E$52,1)</f>
+      <c r="F39">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G39">
@@ -3463,15 +4611,15 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
-        <f>H39-G39</f>
+        <f t="shared" si="11"/>
         <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.16168630757756886</v>
       </c>
       <c r="K39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L39">
@@ -3481,15 +4629,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -3504,15 +4652,15 @@
         <v>37565141.859999903</v>
       </c>
       <c r="D40">
-        <f>C40-B40</f>
+        <f t="shared" si="9"/>
         <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
-        <f>IFERROR(D40/B40,0)</f>
+        <f t="shared" si="10"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40" s="9">
-        <f>RANK(E40,$E$2:$E$52,1)</f>
+      <c r="F40">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G40">
@@ -3522,15 +4670,15 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
-        <f>H40-G40</f>
+        <f t="shared" si="11"/>
         <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.9078567313795014E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="L40">
@@ -3540,15 +4688,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
     </row>
@@ -3563,15 +4711,15 @@
         <v>4409060.2099999897</v>
       </c>
       <c r="D41">
-        <f>C41-B41</f>
+        <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
-        <f>IFERROR(D41/B41,0)</f>
+        <f t="shared" si="10"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41" s="9">
-        <f>RANK(E41,$E$2:$E$52,1)</f>
+      <c r="F41">
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="G41">
@@ -3581,15 +4729,15 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
-        <f>H41-G41</f>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-2.6927997186112485E-2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="L41">
@@ -3599,15 +4747,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
     </row>
@@ -3622,15 +4770,15 @@
         <v>188551675.67999899</v>
       </c>
       <c r="D42">
-        <f>C42-B42</f>
+        <f t="shared" si="9"/>
         <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
-        <f>IFERROR(D42/B42,0)</f>
+        <f t="shared" si="10"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42" s="9">
-        <f>RANK(E42,$E$2:$E$52,1)</f>
+      <c r="F42">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="G42">
@@ -3640,15 +4788,15 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
-        <f>H42-G42</f>
+        <f t="shared" si="11"/>
         <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1.2072202931945403E-2</v>
       </c>
       <c r="K42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="L42">
@@ -3658,15 +4806,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
     </row>
@@ -3681,15 +4829,15 @@
         <v>7968645.8300000001</v>
       </c>
       <c r="D43">
-        <f>C43-B43</f>
+        <f t="shared" si="9"/>
         <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
-        <f>IFERROR(D43/B43,0)</f>
+        <f t="shared" si="10"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43" s="9">
-        <f>RANK(E43,$E$2:$E$52,1)</f>
+      <c r="F43">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G43">
@@ -3699,15 +4847,15 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
-        <f>H43-G43</f>
+        <f t="shared" si="11"/>
         <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.764477918386123E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="L43">
@@ -3717,15 +4865,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
     </row>
@@ -3740,15 +4888,15 @@
         <v>29789104.379999999</v>
       </c>
       <c r="D44">
-        <f>C44-B44</f>
+        <f t="shared" si="9"/>
         <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
-        <f>IFERROR(D44/B44,0)</f>
+        <f t="shared" si="10"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44" s="9">
-        <f>RANK(E44,$E$2:$E$52,1)</f>
+      <c r="F44">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="G44">
@@ -3758,15 +4906,15 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
-        <f>H44-G44</f>
+        <f t="shared" si="11"/>
         <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-8.0207454096728314E-3</v>
       </c>
       <c r="K44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="L44">
@@ -3776,15 +4924,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
     </row>
@@ -3799,15 +4947,15 @@
         <v>54589584.0499999</v>
       </c>
       <c r="D45">
-        <f>C45-B45</f>
+        <f t="shared" si="9"/>
         <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
-        <f>IFERROR(D45/B45,0)</f>
+        <f t="shared" si="10"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45" s="9">
-        <f>RANK(E45,$E$2:$E$52,1)</f>
+      <c r="F45">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="G45">
@@ -3817,15 +4965,15 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
-        <f>H45-G45</f>
+        <f t="shared" si="11"/>
         <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.0246320962372462E-2</v>
       </c>
       <c r="K45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="L45">
@@ -3835,15 +4983,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
     </row>
@@ -3858,15 +5006,15 @@
         <v>258322.43</v>
       </c>
       <c r="D46">
-        <f>C46-B46</f>
+        <f t="shared" si="9"/>
         <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
-        <f>IFERROR(D46/B46,0)</f>
+        <f t="shared" si="10"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46" s="9">
-        <f>RANK(E46,$E$2:$E$52,1)</f>
+      <c r="F46">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="G46">
@@ -3876,15 +5024,15 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
-        <f>H46-G46</f>
+        <f t="shared" si="11"/>
         <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-3.3399350458007716E-2</v>
       </c>
       <c r="K46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="L46">
@@ -3894,15 +5042,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
     </row>
@@ -3917,15 +5065,15 @@
         <v>70378426.719999999</v>
       </c>
       <c r="D47">
-        <f>C47-B47</f>
+        <f t="shared" si="9"/>
         <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
-        <f>IFERROR(D47/B47,0)</f>
+        <f t="shared" si="10"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47" s="9">
-        <f>RANK(E47,$E$2:$E$52,1)</f>
+      <c r="F47">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="G47">
@@ -3935,15 +5083,15 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
-        <f>H47-G47</f>
+        <f t="shared" si="11"/>
         <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-3.330268730789944E-4</v>
       </c>
       <c r="K47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="L47">
@@ -3953,15 +5101,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
     </row>
@@ -3976,15 +5124,15 @@
         <v>6527352.5699999901</v>
       </c>
       <c r="D48">
-        <f>C48-B48</f>
+        <f t="shared" si="9"/>
         <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
-        <f>IFERROR(D48/B48,0)</f>
+        <f t="shared" si="10"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48" s="9">
-        <f>RANK(E48,$E$2:$E$52,1)</f>
+      <c r="F48">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G48">
@@ -3994,15 +5142,15 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
-        <f>H48-G48</f>
+        <f t="shared" si="11"/>
         <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-4.2274540964939038E-2</v>
       </c>
       <c r="K48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="L48">
@@ -4012,15 +5160,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -4035,15 +5183,15 @@
         <v>90499.43</v>
       </c>
       <c r="D49">
-        <f>C49-B49</f>
+        <f t="shared" si="9"/>
         <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
-        <f>IFERROR(D49/B49,0)</f>
+        <f t="shared" si="10"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49" s="9">
-        <f>RANK(E49,$E$2:$E$52,1)</f>
+      <c r="F49">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="G49">
@@ -4053,15 +5201,15 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
-        <f>H49-G49</f>
+        <f t="shared" si="11"/>
         <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-7.4718268785991485E-2</v>
       </c>
       <c r="K49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="L49">
@@ -4071,15 +5219,15 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -4094,15 +5242,15 @@
         <v>832600</v>
       </c>
       <c r="D50">
-        <f>C50-B50</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f>IFERROR(D50/B50,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F50" s="9">
-        <f>RANK(E50,$E$2:$E$52,1)</f>
+      <c r="F50">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G50">
@@ -4112,15 +5260,15 @@
         <v>859100</v>
       </c>
       <c r="I50">
-        <f>H50-G50</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L50">
@@ -4130,15 +5278,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -4153,15 +5301,15 @@
         <v>8499425.3399999905</v>
       </c>
       <c r="D51">
-        <f>C51-B51</f>
+        <f t="shared" si="9"/>
         <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
-        <f>IFERROR(D51/B51,0)</f>
+        <f t="shared" si="10"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51" s="9">
-        <f>RANK(E51,$E$2:$E$52,1)</f>
+      <c r="F51">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="G51">
@@ -4171,15 +5319,15 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
-        <f>H51-G51</f>
+        <f t="shared" si="11"/>
         <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-3.796233476981066E-2</v>
       </c>
       <c r="K51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="L51">
@@ -4189,15 +5337,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
     </row>
@@ -4212,15 +5360,15 @@
         <v>2254684.7999999998</v>
       </c>
       <c r="D52">
-        <f>C52-B52</f>
+        <f t="shared" si="9"/>
         <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
-        <f>IFERROR(D52/B52,0)</f>
+        <f t="shared" si="10"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52" s="9">
-        <f>RANK(E52,$E$2:$E$52,1)</f>
+      <c r="F52">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G52">
@@ -4230,15 +5378,15 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
-        <f>H52-G52</f>
+        <f t="shared" si="11"/>
         <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-0.10705766018222174</v>
       </c>
       <c r="K52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L52">
@@ -4248,15 +5396,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -4283,16 +5431,14 @@
       <c r="A56" t="s">
         <v>24</v>
       </c>
-      <c r="B56">
-        <f>VLOOKUP(A56,$A$2:$P$52,4,FALSE)</f>
+      <c r="B56" cm="1">
+        <f t="array" ref="B56:D56">VLOOKUP(A56,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56,$A$2:$P$52,9,FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56,$A$2:$P$52,14,FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4300,16 +5446,14 @@
       <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57">
-        <f t="shared" ref="B57:B61" si="5">VLOOKUP(A57,$A$2:$P$52,4,FALSE)</f>
+      <c r="B57" cm="1">
+        <f t="array" ref="B57:D57">VLOOKUP(A57,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="6">VLOOKUP(A57,$A$2:$P$52,9,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="7">VLOOKUP(A57,$A$2:$P$52,14,FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4317,16 +5461,14 @@
       <c r="A58" t="s">
         <v>32</v>
       </c>
-      <c r="B58">
-        <f t="shared" si="5"/>
+      <c r="B58" cm="1">
+        <f t="array" ref="B58:D58">VLOOKUP(A58,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="6"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="7"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4334,16 +5476,14 @@
       <c r="A59" t="s">
         <v>38</v>
       </c>
-      <c r="B59">
-        <f t="shared" si="5"/>
+      <c r="B59" cm="1">
+        <f t="array" ref="B59:D59">VLOOKUP(A59,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="6"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="7"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4351,16 +5491,14 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60">
-        <f t="shared" si="5"/>
+      <c r="B60" cm="1">
+        <f t="array" ref="B60:D60">VLOOKUP(A60,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="6"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="7"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4368,16 +5506,14 @@
       <c r="A61" t="s">
         <v>55</v>
       </c>
-      <c r="B61">
-        <f t="shared" si="5"/>
+      <c r="B61" cm="1">
+        <f t="array" ref="B61:D61">VLOOKUP(A61,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="6"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="7"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4422,15 +5558,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="8">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="9">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="10">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4439,15 +5575,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4456,15 +5592,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4473,15 +5609,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="9"/>
+        <f>_xlfn.XLOOKUP(A69,$A$2:$A$52,$I$2:$I$52)</f>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4490,15 +5626,15 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4543,15 +5679,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="11">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f>INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="12">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="15">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="13">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="16">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4560,15 +5696,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B76:B79" si="17">INDEX($D$2:$D$52,MATCH(A76,$A$2:$A$52,0))</f>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4577,15 +5713,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4594,15 +5730,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4611,15 +5747,15 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4640,6 +5776,9 @@
       <c r="C83" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="D83" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -4647,11 +5786,15 @@
       </c>
       <c r="B84" s="6">
         <f>IFERROR(INDEX($B$2:$B$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>356640100</v>
+        <v>7670700</v>
       </c>
       <c r="C84" s="6">
         <f>IFERROR(INDEX($C$2:$C$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>341243679.13</v>
+        <v>6947552.6699999999</v>
+      </c>
+      <c r="D84" s="6">
+        <f>C84-B84</f>
+        <v>-723147.33000000007</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -4660,11 +5803,15 @@
       </c>
       <c r="B85" s="6">
         <f>IFERROR(INDEX($G$2:$G$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>382685200</v>
+        <v>7968300</v>
       </c>
       <c r="C85" s="6">
         <f>IFERROR(INDEX($H$2:$H$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>346340810.81999999</v>
+        <v>7020609.3200000003</v>
+      </c>
+      <c r="D85" s="6">
+        <f t="shared" ref="D85:D86" si="18">C85-B85</f>
+        <v>-947690.6799999997</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -4673,16 +5820,20 @@
       </c>
       <c r="B86" s="6">
         <f>IFERROR(INDEX($L$2:$L$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>376548600</v>
+        <v>7759600</v>
       </c>
       <c r="C86" s="6">
         <f>IFERROR(INDEX($M$2:$M$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>355279492.22999901</v>
+        <v>7497322.9100000001</v>
+      </c>
+      <c r="D86" s="6">
+        <f t="shared" si="18"/>
+        <v>-262277.08999999985</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -4706,7 +5857,7 @@
         <v>2</v>
       </c>
       <c r="E89" s="7"/>
-      <c r="F89" s="10">
+      <c r="F89" s="7">
         <v>3</v>
       </c>
     </row>
@@ -4723,7 +5874,7 @@
       <c r="E90" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="F90" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G90" s="8" t="s">
@@ -4734,7 +5885,14 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP(INDEX($A$2:$A$52,MATCH(MIN($F$2:$F$52),$F$2:$F$52,0)),$A$2:$A$52,$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5">
+        <f>_xlfn.XLOOKUP(INDEX($A$2:$A$52,MATCH(MIN($F$2:$F$52),F2:F52,0)),$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
       <c r="E91" s="5"/>
       <c r="G91" s="5"/>
     </row>
@@ -4742,7 +5900,6 @@
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
       <c r="E92" s="5"/>
       <c r="G92" s="5"/>
     </row>
@@ -4750,7 +5907,6 @@
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
       <c r="E93" s="5"/>
       <c r="G93" s="5"/>
     </row>
@@ -4771,7 +5927,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="7"/>
-      <c r="F96" s="10">
+      <c r="F96" s="7">
         <v>3</v>
       </c>
     </row>
@@ -4788,7 +5944,7 @@
       <c r="E97" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="11" t="s">
+      <c r="F97" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G97" s="8" t="s">
@@ -4808,7 +5964,6 @@
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
       <c r="E99" s="4"/>
       <c r="G99" s="4"/>
       <c r="I99" s="4"/>
@@ -4821,6 +5976,11 @@
       <c r="E100" s="4"/>
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F52">
@@ -4833,6 +5993,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4841,7 +6002,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Lookup excel push Sept 19 11:21 pm
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,21 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\Documents\NSS-DA13\Excel\lookups-exercise-RenukaD13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD8B44A-EDB5-4FBF-8008-3119B2E87921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD79B4-EECE-4D96-8F40-46500AE4F418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">metro_budget!$A$84:$A$87</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">metro_budget!$B$83</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">metro_budget!$B$84:$B$87</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">metro_budget!$C$83</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">metro_budget!$C$84:$C$87</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,30 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="92">
   <si>
     <t>Department</t>
   </si>
@@ -336,6 +307,9 @@
   </si>
   <si>
     <t>Diffrence</t>
+  </si>
+  <si>
+    <t>Bonus Qust-7</t>
   </si>
 </sst>
 </file>
@@ -494,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,6 +654,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -841,7 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -853,6 +833,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -967,7 +950,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Administrative Budget and Actual amount for fiscal years. </a:t>
+              <a:t>Budget and Actual amount for fiscal years. </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1061,7 +1044,7 @@
                   <c:v>FY19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Assessor of Property</c:v>
+                  <c:v>Clerk and Master - Chancery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1073,13 +1056,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7670700</c:v>
+                  <c:v>1552100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7968300</c:v>
+                  <c:v>1590700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7759600</c:v>
+                  <c:v>1579300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1129,7 +1112,7 @@
                   <c:v>FY19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Assessor of Property</c:v>
+                  <c:v>Clerk and Master - Chancery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1141,13 +1124,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6947552.6699999999</c:v>
+                  <c:v>1315623.30999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7020609.3200000003</c:v>
+                  <c:v>1383905.98999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7497322.9100000001</c:v>
+                  <c:v>1337735.3199999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,7 +1198,7 @@
                   <c:v>FY19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Assessor of Property</c:v>
+                  <c:v>Clerk and Master - Chancery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1227,13 +1210,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-723147.33000000007</c:v>
+                  <c:v>-236476.69000000996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-947690.6799999997</c:v>
+                  <c:v>-206794.01000001002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-262277.08999999985</c:v>
+                  <c:v>-241564.68000000995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1997,14 +1980,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1044575</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>11112</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>36512</xdr:rowOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>68262</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2331,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5412,6 +5395,9 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="E54" s="9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
@@ -5424,6 +5410,15 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5431,14 +5426,28 @@
       <c r="A56" t="s">
         <v>24</v>
       </c>
-      <c r="B56" cm="1">
-        <f t="array" ref="B56:D56">VLOOKUP(A56,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B56">
+        <f>VLOOKUP($A56,$A$1:$P$52,4,FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
+        <f>VLOOKUP($A56,$A$1:$P$52,9,FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
+        <f>VLOOKUP($A56,$A$1:$P$52,14,FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="E56" s="10">
+        <f>VLOOKUP($A56,$A$1:$P$52,MATCH(B$55,$1:$1,0),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="F56" s="10">
+        <f t="shared" ref="F56:G61" si="12">VLOOKUP($A56,$A$1:$P$52,MATCH(C$55,$1:$1,0),FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="G56" s="10">
+        <f t="shared" si="12"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5446,14 +5455,28 @@
       <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57" cm="1">
-        <f t="array" ref="B57:D57">VLOOKUP(A57,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B57">
+        <f t="shared" ref="B57:B61" si="13">VLOOKUP($A57,$A$1:$P$52,4,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
+        <f t="shared" ref="C57:C61" si="14">VLOOKUP($A57,$A$1:$P$52,9,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
+        <f t="shared" ref="D57:D61" si="15">VLOOKUP($A57,$A$1:$P$52,14,FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="E57" s="10">
+        <f t="shared" ref="E57:E61" si="16">VLOOKUP($A57,$A$1:$P$52,MATCH(B$55,$1:$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G57" s="10">
+        <f t="shared" si="12"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5461,14 +5484,28 @@
       <c r="A58" t="s">
         <v>32</v>
       </c>
-      <c r="B58" cm="1">
-        <f t="array" ref="B58:D58">VLOOKUP(A58,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B58">
+        <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
+        <f t="shared" si="14"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
+        <f t="shared" si="15"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="E58" s="10">
+        <f t="shared" si="16"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="F58" s="10">
+        <f t="shared" si="12"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="G58" s="10">
+        <f t="shared" si="12"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5476,14 +5513,28 @@
       <c r="A59" t="s">
         <v>38</v>
       </c>
-      <c r="B59" cm="1">
-        <f t="array" ref="B59:D59">VLOOKUP(A59,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B59">
+        <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
+        <f t="shared" si="14"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
+        <f t="shared" si="15"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="E59" s="10">
+        <f t="shared" si="16"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="F59" s="10">
+        <f t="shared" si="12"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="G59" s="10">
+        <f t="shared" si="12"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5491,14 +5542,28 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" cm="1">
-        <f t="array" ref="B60:D60">VLOOKUP(A60,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B60">
+        <f t="shared" si="13"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
+        <f t="shared" si="14"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
+        <f t="shared" si="15"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="E60" s="10">
+        <f t="shared" si="16"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="F60" s="10">
+        <f t="shared" si="12"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="G60" s="10">
+        <f t="shared" si="12"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5506,14 +5571,28 @@
       <c r="A61" t="s">
         <v>55</v>
       </c>
-      <c r="B61" cm="1">
-        <f t="array" ref="B61:D61">VLOOKUP(A61,$A$2:$P$52,MATCH($B$55:$D$55,metro_budget!$A$1:$P$1),FALSE)</f>
+      <c r="B61">
+        <f t="shared" si="13"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
+        <f t="shared" si="14"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
+        <f t="shared" si="15"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="E61" s="10">
+        <f t="shared" si="16"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="F61" s="10">
+        <f t="shared" si="12"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="G61" s="10">
+        <f t="shared" si="12"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5535,8 +5614,11 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5553,63 +5635,63 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="17">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="18">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="19">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
@@ -5617,33 +5699,36 @@
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E72" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5656,8 +5741,17 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5673,8 +5767,20 @@
         <f>INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E74" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A52,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="F74" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A52,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="G74" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -5683,79 +5789,139 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="15">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="20">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="16">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="21">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E75" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A75,$A$2:$A53,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F75" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A75,$A$2:$A53,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A75,$A$2:$A53,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" ref="B76:B79" si="17">INDEX($D$2:$D$52,MATCH(A76,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B76:B79" si="22">INDEX($D$2:$D$52,MATCH(A76,$A$2:$A$52,0))</f>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E76" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A76,$A$2:$A54,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="F76" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A76,$A$2:$A54,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="G76" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A76,$A$2:$A54,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E77" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A77,$A$2:$A55,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="F77" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A77,$A$2:$A55,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="G77" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A77,$A$2:$A55,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E78" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A78,$A$2:$A56,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="F78" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A78,$A$2:$A56,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="G78" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A78,$A$2:$A56,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="E79" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A79,$A$2:$A57,0),MATCH(E$73,$A$1:$P$1,0))</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="F79" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A79,$A$2:$A57,0),MATCH(F$73,$A$1:$P$1,0))</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="G79" s="10">
+        <f>INDEX($A$2:$P$52,MATCH($A79,$A$2:$A57,0),MATCH(G$73,$A$1:$P$1,0))</f>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5786,15 +5952,15 @@
       </c>
       <c r="B84" s="6">
         <f>IFERROR(INDEX($B$2:$B$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>7670700</v>
+        <v>1552100</v>
       </c>
       <c r="C84" s="6">
         <f>IFERROR(INDEX($C$2:$C$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>6947552.6699999999</v>
+        <v>1315623.30999999</v>
       </c>
       <c r="D84" s="6">
         <f>C84-B84</f>
-        <v>-723147.33000000007</v>
+        <v>-236476.69000000996</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -5803,15 +5969,15 @@
       </c>
       <c r="B85" s="6">
         <f>IFERROR(INDEX($G$2:$G$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>7968300</v>
+        <v>1590700</v>
       </c>
       <c r="C85" s="6">
         <f>IFERROR(INDEX($H$2:$H$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>7020609.3200000003</v>
+        <v>1383905.98999999</v>
       </c>
       <c r="D85" s="6">
-        <f t="shared" ref="D85:D86" si="18">C85-B85</f>
-        <v>-947690.6799999997</v>
+        <f t="shared" ref="D85:D86" si="23">C85-B85</f>
+        <v>-206794.01000001002</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -5820,20 +5986,20 @@
       </c>
       <c r="B86" s="6">
         <f>IFERROR(INDEX($L$2:$L$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>7759600</v>
+        <v>1579300</v>
       </c>
       <c r="C86" s="6">
         <f>IFERROR(INDEX($M$2:$M$52,MATCH($A$87,$A$2:$A$52,0)),"Select Department")</f>
-        <v>7497322.9100000001</v>
+        <v>1337735.3199999901</v>
       </c>
       <c r="D86" s="6">
-        <f t="shared" si="18"/>
-        <v>-262277.08999999985</v>
+        <f t="shared" si="23"/>
+        <v>-241564.68000000995</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -5986,7 +6152,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F52">
     <sortCondition ref="F2:F52"/>
   </sortState>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 A87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Lookup exercise final push 6-Oct 6:02 PM
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\Documents\NSS-DA13\Excel\lookups-exercise-RenukaD13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD79B4-EECE-4D96-8F40-46500AE4F418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B4F6D2-2477-4BB5-A074-30EA6567AE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -320,7 +320,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +466,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -835,7 +842,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1980,14 +1987,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1044575</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>68262</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2314,8 +2321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2393,7 +2400,7 @@
         <v>341243679.13</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="0">C2-B2</f>
+        <f>C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
@@ -2411,7 +2418,7 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I33" si="1">H2-G2</f>
+        <f t="shared" ref="I2:I33" si="0">H2-G2</f>
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
@@ -2456,11 +2463,11 @@
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E33" si="2">IFERROR(D3/B3,0)</f>
+        <f t="shared" ref="E3:E33" si="1">IFERROR(D3/B3,0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="3">_xlfn.RANK.EQ(E3,$E$2:$E$52,1)</f>
+        <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3,$E$2:$E$52,1)</f>
         <v>22</v>
       </c>
       <c r="G3">
@@ -2470,15 +2477,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/H3,0)</f>
+        <f t="shared" ref="J3:J52" si="3">IFERROR(I3/H3,0)</f>
         <v>-7.1587313673678488E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3,$J$2:$J$52,1)</f>
+        <f t="shared" ref="K3:K52" si="4">_xlfn.RANK.EQ(J3,$J$2:$J$52,1)</f>
         <v>14</v>
       </c>
       <c r="L3">
@@ -2488,15 +2495,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="6">M3-L3</f>
+        <f t="shared" ref="N3:N52" si="5">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,0)</f>
+        <f t="shared" ref="O3:O52" si="6">IFERROR(N3/L3,0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3,$O$2:$O$52,1)</f>
+        <f t="shared" ref="P3:P52" si="7">_xlfn.RANK.EQ(O3,$O$2:$O$52,1)</f>
         <v>37</v>
       </c>
     </row>
@@ -2511,15 +2518,15 @@
         <v>3115157.5599999898</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2:D33" si="8">C4-B4</f>
         <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.9327413275443007E-3</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="2"/>
-        <v>-4.9327413275443007E-3</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="G4">
@@ -2529,15 +2536,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.7440707697694863E-2</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="4"/>
-        <v>-1.7440707697694863E-2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L4">
@@ -2547,15 +2554,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
+        <f t="shared" si="5"/>
+        <v>-97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
         <f t="shared" si="6"/>
-        <v>-97416.950000009965</v>
-      </c>
-      <c r="O4" s="5">
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="7"/>
-        <v>-2.6599210899959033E-2</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="8"/>
         <v>25</v>
       </c>
     </row>
@@ -2570,15 +2577,15 @@
         <v>6947552.6699999999</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>-9.4273968477453174E-2</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="2"/>
-        <v>-9.4273968477453174E-2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G5">
@@ -2588,15 +2595,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.13498695580457107</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="4"/>
-        <v>-0.13498695580457107</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L5">
@@ -2606,15 +2613,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
+        <f t="shared" si="5"/>
+        <v>-262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
         <f t="shared" si="6"/>
-        <v>-262277.08999999985</v>
-      </c>
-      <c r="O5" s="5">
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="7"/>
-        <v>-3.3800336357544182E-2</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="8"/>
         <v>22</v>
       </c>
     </row>
@@ -2629,15 +2636,15 @@
         <v>385908.52</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>-5.7149963352064452E-2</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="2"/>
-        <v>-5.7149963352064452E-2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G6">
@@ -2647,15 +2654,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.7331268866947632E-3</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="4"/>
-        <v>-1.7331268866947632E-3</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="L6">
@@ -2665,15 +2672,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
+        <f t="shared" si="5"/>
+        <v>-85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
         <f t="shared" si="6"/>
-        <v>-85.710000001010485</v>
-      </c>
-      <c r="O6" s="5">
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="7"/>
-        <v>-1.925202156356929E-4</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="8"/>
         <v>39</v>
       </c>
     </row>
@@ -2688,15 +2695,15 @@
         <v>2946071.21</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="2"/>
-        <v>-0.11502817362571344</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G7">
@@ -2706,15 +2713,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11123002959403271</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="4"/>
-        <v>-0.11123002959403271</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L7">
@@ -2724,15 +2731,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
+        <f t="shared" si="5"/>
+        <v>-398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
         <f t="shared" si="6"/>
-        <v>-398759.91999999993</v>
-      </c>
-      <c r="O7" s="5">
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="7"/>
-        <v>-0.11920361114432618</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -2747,15 +2754,15 @@
         <v>1315623.30999999</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="2"/>
-        <v>-0.15235918433091292</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -2765,15 +2772,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.14942778736004425</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="4"/>
-        <v>-0.14942778736004425</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L8">
@@ -2783,15 +2790,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
+        <f t="shared" si="5"/>
+        <v>-241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
         <f t="shared" si="6"/>
-        <v>-241564.68000000995</v>
-      </c>
-      <c r="O8" s="5">
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="7"/>
-        <v>-0.15295680364719175</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2806,15 +2813,15 @@
         <v>8952825.2799999993</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.2417130511048909E-2</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="2"/>
-        <v>-4.2417130511048909E-2</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G9">
@@ -2824,15 +2831,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11528186307014912</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="4"/>
-        <v>-0.11528186307014912</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L9">
@@ -2842,15 +2849,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
+        <f t="shared" si="5"/>
+        <v>-796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
         <f t="shared" si="6"/>
-        <v>-796900.47000000998</v>
-      </c>
-      <c r="O9" s="5">
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="7"/>
-        <v>-7.3852043000788653E-2</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -2865,15 +2872,15 @@
         <v>407090.37</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>-8.1681998646514792E-2</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="2"/>
-        <v>-8.1681998646514792E-2</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G10">
@@ -2883,15 +2890,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.8328067339072524E-2</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="4"/>
-        <v>-5.8328067339072524E-2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="L10">
@@ -2901,15 +2908,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
+        <f t="shared" si="5"/>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
         <f t="shared" si="6"/>
-        <v>-9181.0800000000163</v>
-      </c>
-      <c r="O10" s="5">
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="7"/>
-        <v>-1.883298461538465E-2</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="8"/>
         <v>29</v>
       </c>
     </row>
@@ -2924,33 +2931,33 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="J11" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L11">
@@ -2960,15 +2967,15 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
+        <f t="shared" si="5"/>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="O11" s="5">
         <f t="shared" si="6"/>
-        <v>-311228.08999999997</v>
-      </c>
-      <c r="O11" s="5">
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="7"/>
-        <v>-0.82994157333333329</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -2983,15 +2990,15 @@
         <v>4066595.33</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>-5.0060657805601608E-2</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="2"/>
-        <v>-5.0060657805601608E-2</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="G12">
@@ -3001,15 +3008,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.11766445318188171</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="4"/>
-        <v>-0.11766445318188171</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L12">
@@ -3019,15 +3026,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
         <f t="shared" si="6"/>
-        <v>-306086.86000000034</v>
-      </c>
-      <c r="O12" s="5">
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="7"/>
-        <v>-6.5433934755654441E-2</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -3042,15 +3049,15 @@
         <v>5772288.3300000001</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.2912833886247806E-2</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="2"/>
-        <v>-1.2912833886247806E-2</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="G13">
@@ -3060,15 +3067,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.3243850088734883E-2</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="4"/>
-        <v>-5.3243850088734883E-2</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="L13">
@@ -3078,15 +3085,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
         <f t="shared" si="6"/>
-        <v>-150323.33000000007</v>
-      </c>
-      <c r="O13" s="5">
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="7"/>
-        <v>-2.4217184605222895E-2</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="8"/>
         <v>27</v>
       </c>
     </row>
@@ -3101,15 +3108,15 @@
         <v>505017.37</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.3637949218750009E-2</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="2"/>
-        <v>-1.3637949218750009E-2</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="G14">
@@ -3119,15 +3126,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.1626592968636483E-2</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="4"/>
-        <v>-1.1626592968636483E-2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="L14">
@@ -3137,15 +3144,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
+        <f t="shared" si="5"/>
+        <v>-21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
         <f t="shared" si="6"/>
-        <v>-21210.119999999995</v>
-      </c>
-      <c r="O14" s="5">
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="7"/>
-        <v>-4.0308095781071827E-2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="8"/>
         <v>19</v>
       </c>
     </row>
@@ -3160,15 +3167,15 @@
         <v>156545919.90000001</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="2"/>
-        <v>3.1837408866824991E-3</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="G15">
@@ -3178,15 +3185,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.6607825420280143E-2</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="4"/>
-        <v>-4.6607825420280143E-2</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L15">
@@ -3196,15 +3203,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
+        <f t="shared" si="5"/>
+        <v>-4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
         <f t="shared" si="6"/>
-        <v>-4502589.1500009894</v>
-      </c>
-      <c r="O15" s="5">
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="7"/>
-        <v>-2.3829085727446114E-2</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="8"/>
         <v>28</v>
       </c>
     </row>
@@ -3219,15 +3226,15 @@
         <v>6522480.4599999897</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.1850188616360429E-2</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="2"/>
-        <v>-1.1850188616360429E-2</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="G16">
@@ -3237,15 +3244,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.7697842991158804E-4</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="4"/>
-        <v>-2.7697842991158804E-4</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="L16">
@@ -3255,15 +3262,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-107</v>
+      </c>
+      <c r="O16" s="5">
         <f t="shared" si="6"/>
-        <v>-107</v>
-      </c>
-      <c r="O16" s="5">
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="7"/>
-        <v>-1.4464932677229222E-5</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="8"/>
         <v>43</v>
       </c>
     </row>
@@ -3278,15 +3285,15 @@
         <v>14439480.050000001</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.8351094826658003E-2</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="2"/>
-        <v>-2.8351094826658003E-2</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="G17">
@@ -3296,15 +3303,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.5370836152683523E-2</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="4"/>
-        <v>-4.5370836152683523E-2</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="L17">
@@ -3314,15 +3321,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
+        <f t="shared" si="5"/>
+        <v>-965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
         <f t="shared" si="6"/>
-        <v>-965742.96000000089</v>
-      </c>
-      <c r="O17" s="5">
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="7"/>
-        <v>-6.3071811282801551E-2</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -3337,15 +3344,15 @@
         <v>2615303.8999999901</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>-5.4037002206391245E-2</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="2"/>
-        <v>-5.4037002206391245E-2</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G18">
@@ -3355,15 +3362,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>-7.0835350460006705E-2</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="4"/>
-        <v>-7.0835350460006705E-2</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="L18">
@@ -3373,15 +3380,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
+        <f t="shared" si="5"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
         <f t="shared" si="6"/>
-        <v>-374962.91000000015</v>
-      </c>
-      <c r="O18" s="5">
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="7"/>
-        <v>-0.12882667147667154</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -3396,15 +3403,15 @@
         <v>8460963.1999999899</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.258504294298146E-2</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="2"/>
-        <v>-4.258504294298146E-2</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="G19">
@@ -3414,15 +3421,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.0250917955821899E-2</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="4"/>
-        <v>-8.0250917955821899E-2</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="L19">
@@ -3432,15 +3439,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
         <f t="shared" si="6"/>
-        <v>-576344.08999999985</v>
-      </c>
-      <c r="O19" s="5">
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="7"/>
-        <v>-6.1687262121374278E-2</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -3455,15 +3462,15 @@
         <v>124384360.159999</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.2379538203300809E-5</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="2"/>
-        <v>-1.2379538203300809E-5</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="G20">
@@ -3473,15 +3480,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
+        <f t="shared" si="3"/>
+        <v>-7.4147890262190919E-5</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="4"/>
-        <v>-7.4147890262190919E-5</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="L20">
@@ -3491,15 +3498,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
         <f t="shared" si="6"/>
-        <v>-116.46000100672245</v>
-      </c>
-      <c r="O20" s="5">
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="7"/>
-        <v>-8.9158438821450736E-7</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="8"/>
         <v>46</v>
       </c>
     </row>
@@ -3514,15 +3521,15 @@
         <v>22408587.5499999</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>-7.9052463618023094E-2</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="2"/>
-        <v>-7.9052463618023094E-2</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G21">
@@ -3532,15 +3539,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.1276787064492179E-2</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="4"/>
-        <v>-8.1276787064492179E-2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="L21">
@@ -3550,15 +3557,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
         <f t="shared" si="6"/>
-        <v>-888926.91000010073</v>
-      </c>
-      <c r="O21" s="5">
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="7"/>
-        <v>-3.6546762734864152E-2</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -3573,15 +3580,15 @@
         <v>11412339.8799999</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.3285502334437123E-2</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="2"/>
-        <v>-1.3285502334437123E-2</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="G22">
@@ -3591,15 +3598,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.6004272606362537E-2</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="4"/>
-        <v>-1.6004272606362537E-2</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="L22">
@@ -3609,15 +3616,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
+        <f t="shared" si="5"/>
+        <v>-745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
         <f t="shared" si="6"/>
-        <v>-745.23000000044703</v>
-      </c>
-      <c r="O22" s="5">
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="7"/>
-        <v>-6.2439674240938325E-5</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="8"/>
         <v>42</v>
       </c>
     </row>
@@ -3632,15 +3639,15 @@
         <v>20036743.4099999</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>-3.9590110100806722E-2</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="2"/>
-        <v>-3.9590110100806722E-2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G23">
@@ -3650,15 +3657,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.4271622872473403E-2</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="4"/>
-        <v>-4.4271622872473403E-2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="L23">
@@ -3668,15 +3675,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
+        <f t="shared" si="5"/>
+        <v>-601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>-601242.55999999866</v>
-      </c>
-      <c r="O23" s="5">
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="7"/>
-        <v>-2.5892971236375011E-2</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="8"/>
         <v>26</v>
       </c>
     </row>
@@ -3691,15 +3698,15 @@
         <v>904969.19</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.3334943305713101E-2</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="2"/>
-        <v>-1.3334943305713101E-2</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="G24">
@@ -3709,15 +3716,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.2620844647132936E-2</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="4"/>
-        <v>-4.2620844647132936E-2</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="L24">
@@ -3727,15 +3734,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
+        <f t="shared" si="5"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
         <f t="shared" si="6"/>
-        <v>-72.879999999888241</v>
-      </c>
-      <c r="O24" s="5">
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="7"/>
-        <v>-6.5504224339284781E-5</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="8"/>
         <v>41</v>
       </c>
     </row>
@@ -3750,15 +3757,15 @@
         <v>479149.53</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.0226130964676661E-2</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="2"/>
-        <v>-1.0226130964676661E-2</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="G25">
@@ -3768,15 +3775,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.6101937309368593E-2</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="4"/>
-        <v>-1.6101937309368593E-2</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="L25">
@@ -3786,15 +3793,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
+        <f t="shared" si="5"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
         <f t="shared" si="6"/>
-        <v>-1724.9000000000233</v>
-      </c>
-      <c r="O25" s="5">
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="7"/>
-        <v>-3.4741188318228064E-3</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="8"/>
         <v>35</v>
       </c>
     </row>
@@ -3809,15 +3816,15 @@
         <v>4801960.08</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>-8.5306091660634673E-2</v>
+      </c>
+      <c r="F26">
         <f t="shared" si="2"/>
-        <v>-8.5306091660634673E-2</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G26">
@@ -3827,15 +3834,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
+        <f t="shared" si="3"/>
+        <v>-6.2446392671501351E-2</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="4"/>
-        <v>-6.2446392671501351E-2</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="L26">
@@ -3845,15 +3852,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
         <f t="shared" si="6"/>
-        <v>-313464.79000000004</v>
-      </c>
-      <c r="O26" s="5">
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="7"/>
-        <v>-5.7720881286022069E-2</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
     </row>
@@ -3868,51 +3875,51 @@
         <v>0</v>
       </c>
       <c r="D27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F27">
+      <c r="J27" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K27">
+        <v>48</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5">
+      <c r="P27">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -3927,15 +3934,15 @@
         <v>1250442.02</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>-9.5782760864849215E-2</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="2"/>
-        <v>-9.5782760864849215E-2</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G28">
@@ -3945,15 +3952,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.20631975443303782</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="4"/>
-        <v>-0.20631975443303782</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L28">
@@ -3963,15 +3970,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
+        <f t="shared" si="5"/>
+        <v>-132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
         <f t="shared" si="6"/>
-        <v>-132614.93999999994</v>
-      </c>
-      <c r="O28" s="5">
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="7"/>
-        <v>-8.6909325643882263E-2</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -3986,15 +3993,15 @@
         <v>2523884.71</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.4800253727847622E-2</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="2"/>
-        <v>-1.4800253727847622E-2</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="G29">
@@ -4004,15 +4011,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.2860872747024777E-2</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="4"/>
-        <v>-4.2860872747024777E-2</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="L29">
@@ -4022,15 +4029,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
+        <f t="shared" si="5"/>
+        <v>-35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
         <f t="shared" si="6"/>
-        <v>-35.330000000074506</v>
-      </c>
-      <c r="O29" s="5">
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="7"/>
-        <v>-1.2225336516860273E-5</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="8"/>
         <v>44</v>
       </c>
     </row>
@@ -4045,15 +4052,15 @@
         <v>12030494.1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
+        <f t="shared" si="1"/>
+        <v>-8.3831374359143746E-3</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="2"/>
-        <v>-8.3831374359143746E-3</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="G30">
@@ -4063,15 +4070,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.971909919295742E-3</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="4"/>
-        <v>-3.971909919295742E-3</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="L30">
@@ -4081,15 +4088,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
+        <f t="shared" si="5"/>
+        <v>-35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
         <f t="shared" si="6"/>
-        <v>-35290.390000000596</v>
-      </c>
-      <c r="O30" s="5">
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="7"/>
-        <v>-2.7439209100169185E-3</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="8"/>
         <v>36</v>
       </c>
     </row>
@@ -4104,15 +4111,15 @@
         <v>1740827.69</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.4030533529678329E-2</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="2"/>
-        <v>-1.4030533529678329E-2</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="G31">
@@ -4122,15 +4129,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.4392662500786743E-2</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="4"/>
-        <v>-3.4392662500786743E-2</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="L31">
@@ -4140,15 +4147,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
+        <f t="shared" si="5"/>
+        <v>-69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
         <f t="shared" si="6"/>
-        <v>-69308.659999999916</v>
-      </c>
-      <c r="O31" s="5">
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="7"/>
-        <v>-3.7049585716576634E-2</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
@@ -4163,15 +4170,15 @@
         <v>5925637.7199999904</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.2294942827617691E-2</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="2"/>
-        <v>-1.2294942827617691E-2</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="G32">
@@ -4181,15 +4188,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.8161839587761623E-2</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="4"/>
-        <v>-1.8161839587761623E-2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="L32">
@@ -4199,15 +4206,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
+        <f t="shared" si="5"/>
+        <v>-169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
         <f t="shared" si="6"/>
-        <v>-169827.98000000045</v>
-      </c>
-      <c r="O32" s="5">
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
         <f t="shared" si="7"/>
-        <v>-2.7581118653977402E-2</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="8"/>
         <v>23</v>
       </c>
     </row>
@@ -4222,15 +4229,15 @@
         <v>920284264.73000002</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
+        <f t="shared" si="1"/>
+        <v>-7.9969930789269058E-3</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="2"/>
-        <v>-7.9969930789269058E-3</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="G33">
@@ -4240,15 +4247,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.6635660489465278E-3</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="4"/>
-        <v>-2.6635660489465278E-3</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="L33">
@@ -4258,15 +4265,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
+        <f t="shared" si="5"/>
+        <v>-5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
         <f t="shared" si="6"/>
-        <v>-5456610.5900000334</v>
-      </c>
-      <c r="O33" s="5">
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="7"/>
-        <v>-5.5141067323084929E-3</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="8"/>
         <v>34</v>
       </c>
     </row>
@@ -4289,7 +4296,7 @@
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="G34">
@@ -4303,11 +4310,11 @@
         <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.1481972192227006E-2</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="4"/>
-        <v>-5.1481972192227006E-2</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="L34">
@@ -4317,15 +4324,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
         <f t="shared" si="6"/>
-        <v>-115798.49000000022</v>
-      </c>
-      <c r="O34" s="5">
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="7"/>
-        <v>-2.6647296115611244E-2</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="8"/>
         <v>24</v>
       </c>
     </row>
@@ -4348,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="G35">
@@ -4362,29 +4369,29 @@
         <v>0</v>
       </c>
       <c r="J35" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K35">
+        <v>48</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="5">
+      <c r="P35">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -4407,7 +4414,7 @@
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G36">
@@ -4421,11 +4428,11 @@
         <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.21287460931962104</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="4"/>
-        <v>-0.21287460931962104</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L36">
@@ -4435,15 +4442,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
+        <f t="shared" si="5"/>
+        <v>-101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
         <f t="shared" si="6"/>
-        <v>-101084.71000000101</v>
-      </c>
-      <c r="O36" s="5">
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
         <f t="shared" si="7"/>
-        <v>-0.11509132414892521</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -4466,7 +4473,7 @@
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="G37">
@@ -4480,11 +4487,11 @@
         <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.2033857953182258E-2</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="4"/>
-        <v>-5.2033857953182258E-2</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="L37">
@@ -4494,15 +4501,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
+        <f t="shared" si="5"/>
+        <v>-188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
         <f t="shared" si="6"/>
-        <v>-188181.66000000015</v>
-      </c>
-      <c r="O37" s="5">
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
         <f t="shared" si="7"/>
-        <v>-8.1928538464887526E-2</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -4525,7 +4532,7 @@
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="G38">
@@ -4539,11 +4546,11 @@
         <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.2223687891129834E-2</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="4"/>
-        <v>-5.2223687891129834E-2</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="L38">
@@ -4553,15 +4560,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
+        <f t="shared" si="5"/>
+        <v>-136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
         <f t="shared" si="6"/>
-        <v>-136.73999999999069</v>
-      </c>
-      <c r="O38" s="5">
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
         <f t="shared" si="7"/>
-        <v>-1.7580354847003174E-4</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="8"/>
         <v>40</v>
       </c>
     </row>
@@ -4584,7 +4591,7 @@
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G39">
@@ -4598,11 +4605,11 @@
         <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.16168630757756886</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="4"/>
-        <v>-0.16168630757756886</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L39">
@@ -4612,15 +4619,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
+        <f t="shared" si="5"/>
+        <v>-79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
         <f t="shared" si="6"/>
-        <v>-79036.1300000099</v>
-      </c>
-      <c r="O39" s="5">
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
         <f t="shared" si="7"/>
-        <v>-4.4919653310605226E-2</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -4643,7 +4650,7 @@
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="G40">
@@ -4657,11 +4664,11 @@
         <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.9078567313795014E-2</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="4"/>
-        <v>-4.9078567313795014E-2</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="L40">
@@ -4671,15 +4678,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
+        <f t="shared" si="5"/>
+        <v>-610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
         <f t="shared" si="6"/>
-        <v>-610436.29000010341</v>
-      </c>
-      <c r="O40" s="5">
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
         <f t="shared" si="7"/>
-        <v>-1.5178676768608648E-2</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="8"/>
         <v>31</v>
       </c>
     </row>
@@ -4702,7 +4709,7 @@
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G41">
@@ -4716,11 +4723,11 @@
         <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
+        <f t="shared" si="3"/>
+        <v>-2.6927997186112485E-2</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="4"/>
-        <v>-2.6927997186112485E-2</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="L41">
@@ -4730,15 +4737,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
+        <f t="shared" si="5"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
         <f t="shared" si="6"/>
-        <v>-82077.349999999627</v>
-      </c>
-      <c r="O41" s="5">
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
         <f t="shared" si="7"/>
-        <v>-1.7099804162586642E-2</v>
-      </c>
-      <c r="P41">
-        <f t="shared" si="8"/>
         <v>30</v>
       </c>
     </row>
@@ -4761,7 +4768,7 @@
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="G42">
@@ -4775,11 +4782,11 @@
         <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.2072202931945403E-2</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="4"/>
-        <v>-1.2072202931945403E-2</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="L42">
@@ -4789,15 +4796,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
+        <f t="shared" si="5"/>
+        <v>-36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
         <f t="shared" si="6"/>
-        <v>-36.250001013278961</v>
-      </c>
-      <c r="O42" s="5">
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
         <f t="shared" si="7"/>
-        <v>-1.8129115815929696E-7</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="8"/>
         <v>47</v>
       </c>
     </row>
@@ -4820,7 +4827,7 @@
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="G43">
@@ -4834,11 +4841,11 @@
         <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.764477918386123E-2</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="4"/>
-        <v>-4.764477918386123E-2</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="L43">
@@ -4848,15 +4855,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
+        <f t="shared" si="5"/>
+        <v>-346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
         <f t="shared" si="6"/>
-        <v>-346517.43000000995</v>
-      </c>
-      <c r="O43" s="5">
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
         <f t="shared" si="7"/>
-        <v>-4.0778750220654303E-2</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="8"/>
         <v>18</v>
       </c>
     </row>
@@ -4879,7 +4886,7 @@
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="G44">
@@ -4893,11 +4900,11 @@
         <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
+        <f t="shared" si="3"/>
+        <v>-8.0207454096728314E-3</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="4"/>
-        <v>-8.0207454096728314E-3</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="L44">
@@ -4907,15 +4914,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
+        <f t="shared" si="5"/>
+        <v>-58.75</v>
+      </c>
+      <c r="O44" s="5">
         <f t="shared" si="6"/>
-        <v>-58.75</v>
-      </c>
-      <c r="O44" s="5">
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
         <f t="shared" si="7"/>
-        <v>-1.8780648419868168E-6</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="8"/>
         <v>45</v>
       </c>
     </row>
@@ -4938,7 +4945,7 @@
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="G45">
@@ -4952,11 +4959,11 @@
         <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.0246320962372462E-2</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="4"/>
-        <v>-4.0246320962372462E-2</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="L45">
@@ -4966,15 +4973,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
+        <f t="shared" si="5"/>
+        <v>-640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
         <f t="shared" si="6"/>
-        <v>-640550.34000010043</v>
-      </c>
-      <c r="O45" s="5">
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="7"/>
-        <v>-1.1432866237947358E-2</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="8"/>
         <v>32</v>
       </c>
     </row>
@@ -4997,7 +5004,7 @@
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="G46">
@@ -5011,11 +5018,11 @@
         <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.3399350458007716E-2</v>
+      </c>
+      <c r="K46">
         <f t="shared" si="4"/>
-        <v>-3.3399350458007716E-2</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="L46">
@@ -5025,15 +5032,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
+        <f t="shared" si="5"/>
+        <v>-12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
         <f t="shared" si="6"/>
-        <v>-12346.840000000986</v>
-      </c>
-      <c r="O46" s="5">
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
         <f t="shared" si="7"/>
-        <v>-4.6225533508053113E-2</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
     </row>
@@ -5056,7 +5063,7 @@
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="G47">
@@ -5070,11 +5077,11 @@
         <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.330268730789944E-4</v>
+      </c>
+      <c r="K47">
         <f t="shared" si="4"/>
-        <v>-3.330268730789944E-4</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="L47">
@@ -5084,15 +5091,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
+        <f t="shared" si="5"/>
+        <v>-21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
         <f t="shared" si="6"/>
-        <v>-21970.820000097156</v>
-      </c>
-      <c r="O47" s="5">
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
         <f t="shared" si="7"/>
-        <v>-2.9266019117572752E-4</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="8"/>
         <v>38</v>
       </c>
     </row>
@@ -5115,7 +5122,7 @@
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G48">
@@ -5129,11 +5136,11 @@
         <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.2274540964939038E-2</v>
+      </c>
+      <c r="K48">
         <f t="shared" si="4"/>
-        <v>-4.2274540964939038E-2</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="L48">
@@ -5143,15 +5150,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
+        <f t="shared" si="5"/>
+        <v>-407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
         <f t="shared" si="6"/>
-        <v>-407449.76000001002</v>
-      </c>
-      <c r="O48" s="5">
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
         <f t="shared" si="7"/>
-        <v>-5.5893132870587676E-2</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -5174,7 +5181,7 @@
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="G49">
@@ -5188,29 +5195,29 @@
         <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
+        <f t="shared" si="3"/>
+        <v>-7.4718268785991485E-2</v>
+      </c>
+      <c r="K49">
         <f t="shared" si="4"/>
-        <v>-7.4718268785991485E-2</v>
-      </c>
-      <c r="K49">
+        <v>13</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="5">
+      <c r="P49">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -5233,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="G50">
@@ -5247,11 +5254,11 @@
         <v>0</v>
       </c>
       <c r="J50" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="L50">
@@ -5261,15 +5268,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="5">
+      <c r="P50">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -5292,7 +5299,7 @@
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="G51">
@@ -5306,11 +5313,11 @@
         <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
+        <f t="shared" si="3"/>
+        <v>-3.796233476981066E-2</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="4"/>
-        <v>-3.796233476981066E-2</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="L51">
@@ -5320,15 +5327,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
+        <f t="shared" si="5"/>
+        <v>-98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
         <f t="shared" si="6"/>
-        <v>-98056.689999999478</v>
-      </c>
-      <c r="O51" s="5">
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="7"/>
-        <v>-1.1100045280114048E-2</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="8"/>
         <v>33</v>
       </c>
     </row>
@@ -5351,7 +5358,7 @@
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G52">
@@ -5365,11 +5372,11 @@
         <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
+        <f t="shared" si="3"/>
+        <v>-0.10705766018222174</v>
+      </c>
+      <c r="K52">
         <f t="shared" si="4"/>
-        <v>-0.10705766018222174</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L52">
@@ -5379,15 +5386,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
+        <f t="shared" si="5"/>
+        <v>-264764.74</v>
+      </c>
+      <c r="O52" s="5">
         <f t="shared" si="6"/>
-        <v>-264764.74</v>
-      </c>
-      <c r="O52" s="5">
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
         <f t="shared" si="7"/>
-        <v>-0.11404408166781529</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -5614,9 +5621,6 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -6138,6 +6142,7 @@
       <c r="A100" t="s">
         <v>75</v>
       </c>
+      <c r="B100" s="11"/>
       <c r="C100" s="4"/>
       <c r="E100" s="4"/>
       <c r="G100" s="4"/>
@@ -6168,7 +6173,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>